<commit_message>
:test_tube: test: funcionalidades para a página 3
</commit_message>
<xml_diff>
--- a/script/.database/Novembro-2024.xlsx
+++ b/script/.database/Novembro-2024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Almoxarifado suprimentos\Suprimentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\PCP\CLAUDIO\VS_CD\dash\DashBoard_cd\script\.database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B6AA41-01BE-4BAF-BB33-E6E95D911C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2196D0-398C-44F4-ACCC-D8661799C58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{206D94FF-8DD9-460F-9052-07E07C6EA2D8}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{206D94FF-8DD9-460F-9052-07E07C6EA2D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -1148,77 +1148,7 @@
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
     <cellStyle name="Vírgula 2 3" xfId="2" xr:uid="{D464673A-692A-4B68-AAA0-4458BA1E072D}"/>
   </cellStyles>
-  <dxfs count="119">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="109">
     <dxf>
       <fill>
         <patternFill>
@@ -2322,11 +2252,11 @@
   <dimension ref="A1:WZG553"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
-      <selection pane="bottomRight" activeCell="W3" sqref="W3"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -2336,8 +2266,8 @@
     <col min="4" max="4" width="70.85546875" style="46" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" style="47" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" style="27" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="10.7109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="27" bestFit="1" customWidth="1"/>
     <col min="10" max="39" width="9.42578125" style="27" customWidth="1"/>
     <col min="40" max="40" width="15.7109375" style="27" customWidth="1"/>
     <col min="41" max="41" width="12.42578125" style="1" customWidth="1"/>
@@ -2868,16 +2798,11 @@
       <c r="AR3" s="25"/>
       <c r="AS3" s="6"/>
       <c r="AT3" s="6"/>
-      <c r="AU3" s="25">
-        <v>12500</v>
-      </c>
+      <c r="AU3" s="25"/>
       <c r="AV3" s="25"/>
       <c r="AW3" s="25"/>
       <c r="AX3" s="25"/>
-      <c r="AY3" s="25">
-        <f>12500+12500</f>
-        <v>25000</v>
-      </c>
+      <c r="AY3" s="25"/>
       <c r="AZ3" s="26"/>
       <c r="BA3" s="6"/>
       <c r="BB3" s="25"/>
@@ -3351,9 +3276,7 @@
       <c r="AZ7" s="26"/>
       <c r="BA7" s="6"/>
       <c r="BB7" s="25"/>
-      <c r="BC7" s="25">
-        <v>1250</v>
-      </c>
+      <c r="BC7" s="25"/>
       <c r="BD7" s="25"/>
       <c r="BE7" s="25"/>
       <c r="BF7" s="25"/>
@@ -3587,9 +3510,7 @@
       <c r="AR9" s="25"/>
       <c r="AS9" s="6"/>
       <c r="AT9" s="6"/>
-      <c r="AU9" s="25">
-        <v>500</v>
-      </c>
+      <c r="AU9" s="25"/>
       <c r="AV9" s="25"/>
       <c r="AW9" s="25"/>
       <c r="AX9" s="25"/>
@@ -3710,9 +3631,7 @@
       <c r="AR10" s="25"/>
       <c r="AS10" s="6"/>
       <c r="AT10" s="6"/>
-      <c r="AU10" s="25">
-        <v>500</v>
-      </c>
+      <c r="AU10" s="25"/>
       <c r="AV10" s="25"/>
       <c r="AW10" s="25"/>
       <c r="AX10" s="25"/>
@@ -3833,9 +3752,7 @@
       <c r="AR11" s="25"/>
       <c r="AS11" s="6"/>
       <c r="AT11" s="6"/>
-      <c r="AU11" s="25">
-        <v>400</v>
-      </c>
+      <c r="AU11" s="25"/>
       <c r="AV11" s="25"/>
       <c r="AW11" s="25"/>
       <c r="AX11" s="25"/>
@@ -3956,9 +3873,7 @@
       <c r="AR12" s="25"/>
       <c r="AS12" s="6"/>
       <c r="AT12" s="6"/>
-      <c r="AU12" s="25">
-        <v>200</v>
-      </c>
+      <c r="AU12" s="25"/>
       <c r="AV12" s="25"/>
       <c r="AW12" s="25"/>
       <c r="AX12" s="25"/>
@@ -4079,9 +3994,7 @@
       <c r="AR13" s="25"/>
       <c r="AS13" s="6"/>
       <c r="AT13" s="6"/>
-      <c r="AU13" s="25">
-        <v>200</v>
-      </c>
+      <c r="AU13" s="25"/>
       <c r="AV13" s="25"/>
       <c r="AW13" s="25"/>
       <c r="AX13" s="25"/>
@@ -4089,9 +4002,7 @@
       <c r="AZ13" s="26"/>
       <c r="BA13" s="6"/>
       <c r="BB13" s="25"/>
-      <c r="BC13" s="25">
-        <v>300</v>
-      </c>
+      <c r="BC13" s="25"/>
       <c r="BD13" s="25"/>
       <c r="BE13" s="25"/>
       <c r="BF13" s="25"/>
@@ -4213,9 +4124,7 @@
       <c r="AZ14" s="26"/>
       <c r="BA14" s="6"/>
       <c r="BB14" s="25"/>
-      <c r="BC14" s="25">
-        <v>300</v>
-      </c>
+      <c r="BC14" s="25"/>
       <c r="BD14" s="25"/>
       <c r="BE14" s="25"/>
       <c r="BF14" s="25"/>
@@ -4440,20 +4349,14 @@
       <c r="AS16" s="6"/>
       <c r="AT16" s="6"/>
       <c r="AU16" s="25"/>
-      <c r="AV16" s="25">
-        <v>12000</v>
-      </c>
+      <c r="AV16" s="25"/>
       <c r="AW16" s="25"/>
       <c r="AX16" s="25"/>
-      <c r="AY16" s="25">
-        <v>12000</v>
-      </c>
+      <c r="AY16" s="25"/>
       <c r="AZ16" s="26"/>
       <c r="BA16" s="6"/>
       <c r="BB16" s="25"/>
-      <c r="BC16" s="25">
-        <v>12600</v>
-      </c>
+      <c r="BC16" s="25"/>
       <c r="BD16" s="25"/>
       <c r="BE16" s="25"/>
       <c r="BF16" s="25"/>
@@ -4910,9 +4813,7 @@
       <c r="AV20" s="25"/>
       <c r="AW20" s="25"/>
       <c r="AX20" s="25"/>
-      <c r="AY20" s="25">
-        <v>5000</v>
-      </c>
+      <c r="AY20" s="25"/>
       <c r="AZ20" s="26"/>
       <c r="BA20" s="6"/>
       <c r="BB20" s="25"/>
@@ -5030,9 +4931,7 @@
       <c r="AY21" s="25"/>
       <c r="AZ21" s="26"/>
       <c r="BA21" s="6"/>
-      <c r="BB21" s="25">
-        <v>1250</v>
-      </c>
+      <c r="BB21" s="25"/>
       <c r="BC21" s="25"/>
       <c r="BD21" s="25"/>
       <c r="BE21" s="25"/>
@@ -5268,9 +5167,7 @@
       <c r="AU23" s="25"/>
       <c r="AV23" s="25"/>
       <c r="AW23" s="25"/>
-      <c r="AX23" s="25">
-        <v>6300</v>
-      </c>
+      <c r="AX23" s="25"/>
       <c r="AY23" s="25"/>
       <c r="AZ23" s="26"/>
       <c r="BA23" s="6"/>
@@ -5504,10 +5401,7 @@
       <c r="BA25" s="6"/>
       <c r="BB25" s="25"/>
       <c r="BC25" s="25"/>
-      <c r="BD25" s="25">
-        <f>15000+15000</f>
-        <v>30000</v>
-      </c>
+      <c r="BD25" s="25"/>
       <c r="BE25" s="25"/>
       <c r="BF25" s="25"/>
       <c r="BG25" s="6"/>
@@ -5981,9 +5875,7 @@
       <c r="AS29" s="6"/>
       <c r="AT29" s="6"/>
       <c r="AU29" s="25"/>
-      <c r="AV29" s="25">
-        <v>12600</v>
-      </c>
+      <c r="AV29" s="25"/>
       <c r="AW29" s="25"/>
       <c r="AX29" s="25"/>
       <c r="AY29" s="25"/>
@@ -5991,9 +5883,7 @@
       <c r="BA29" s="6"/>
       <c r="BB29" s="25"/>
       <c r="BC29" s="25"/>
-      <c r="BD29" s="25">
-        <v>15000</v>
-      </c>
+      <c r="BD29" s="25"/>
       <c r="BE29" s="25"/>
       <c r="BF29" s="25"/>
       <c r="BG29" s="6"/>
@@ -6105,20 +5995,14 @@
       <c r="AR30" s="25"/>
       <c r="AS30" s="6"/>
       <c r="AT30" s="6"/>
-      <c r="AU30" s="25">
-        <v>12600</v>
-      </c>
+      <c r="AU30" s="25"/>
       <c r="AV30" s="25"/>
       <c r="AW30" s="25"/>
-      <c r="AX30" s="25">
-        <v>12600</v>
-      </c>
+      <c r="AX30" s="25"/>
       <c r="AY30" s="25"/>
       <c r="AZ30" s="26"/>
       <c r="BA30" s="6"/>
-      <c r="BB30" s="25">
-        <v>12600</v>
-      </c>
+      <c r="BB30" s="25"/>
       <c r="BC30" s="25"/>
       <c r="BD30" s="25"/>
       <c r="BE30" s="25"/>
@@ -6231,21 +6115,15 @@
       <c r="AS31" s="6"/>
       <c r="AT31" s="6"/>
       <c r="AU31" s="25"/>
-      <c r="AV31" s="25">
-        <v>12600</v>
-      </c>
+      <c r="AV31" s="25"/>
       <c r="AW31" s="25"/>
       <c r="AX31" s="25"/>
-      <c r="AY31" s="25">
-        <v>12600</v>
-      </c>
+      <c r="AY31" s="25"/>
       <c r="AZ31" s="26"/>
       <c r="BA31" s="6"/>
       <c r="BB31" s="25"/>
       <c r="BC31" s="25"/>
-      <c r="BD31" s="25">
-        <v>12600</v>
-      </c>
+      <c r="BD31" s="25"/>
       <c r="BE31" s="25"/>
       <c r="BF31" s="25"/>
       <c r="BG31" s="6"/>
@@ -6358,15 +6236,11 @@
       <c r="AS32" s="6"/>
       <c r="AT32" s="6"/>
       <c r="AU32" s="25"/>
-      <c r="AV32" s="25">
-        <v>12600</v>
-      </c>
+      <c r="AV32" s="25"/>
       <c r="AW32" s="25"/>
       <c r="AX32" s="25"/>
       <c r="AY32" s="25"/>
-      <c r="AZ32" s="25">
-        <v>12500</v>
-      </c>
+      <c r="AZ32" s="25"/>
       <c r="BA32" s="6"/>
       <c r="BB32" s="25"/>
       <c r="BC32" s="25"/>
@@ -6954,19 +6828,13 @@
       <c r="AU37" s="25"/>
       <c r="AV37" s="25"/>
       <c r="AW37" s="25"/>
-      <c r="AX37" s="25">
-        <v>1000</v>
-      </c>
+      <c r="AX37" s="25"/>
       <c r="AY37" s="25"/>
       <c r="AZ37" s="26"/>
       <c r="BA37" s="6"/>
       <c r="BB37" s="25"/>
-      <c r="BC37" s="25">
-        <v>1000</v>
-      </c>
-      <c r="BD37" s="25">
-        <v>1000</v>
-      </c>
+      <c r="BC37" s="25"/>
+      <c r="BD37" s="25"/>
       <c r="BE37" s="25"/>
       <c r="BF37" s="25"/>
       <c r="BG37" s="6"/>
@@ -7206,9 +7074,7 @@
       <c r="BA39" s="6"/>
       <c r="BB39" s="25"/>
       <c r="BC39" s="25"/>
-      <c r="BD39" s="25">
-        <v>150</v>
-      </c>
+      <c r="BD39" s="25"/>
       <c r="BE39" s="25"/>
       <c r="BF39" s="25"/>
       <c r="BG39" s="6"/>
@@ -7444,9 +7310,7 @@
       <c r="BA41" s="6"/>
       <c r="BB41" s="25"/>
       <c r="BC41" s="25"/>
-      <c r="BD41" s="25">
-        <v>150</v>
-      </c>
+      <c r="BD41" s="25"/>
       <c r="BE41" s="25"/>
       <c r="BF41" s="25"/>
       <c r="BG41" s="6"/>
@@ -10859,9 +10723,7 @@
       <c r="AU71" s="25"/>
       <c r="AV71" s="25"/>
       <c r="AW71" s="25"/>
-      <c r="AX71" s="25">
-        <v>301.95</v>
-      </c>
+      <c r="AX71" s="25"/>
       <c r="AY71" s="25"/>
       <c r="AZ71" s="26"/>
       <c r="BA71" s="6"/>
@@ -11322,38 +11184,19 @@
       <c r="AO75" s="24"/>
       <c r="AP75" s="24"/>
       <c r="AQ75" s="24"/>
-      <c r="AR75" s="25">
-        <v>25014</v>
-      </c>
+      <c r="AR75" s="25"/>
       <c r="AS75" s="6"/>
       <c r="AT75" s="6"/>
       <c r="AU75" s="25"/>
       <c r="AV75" s="25"/>
-      <c r="AW75" s="25">
-        <v>29672</v>
-      </c>
-      <c r="AX75" s="25">
-        <f>34022+32942</f>
-        <v>66964</v>
-      </c>
-      <c r="AY75" s="25">
-        <f>34199+33913</f>
-        <v>68112</v>
-      </c>
-      <c r="AZ75" s="25">
-        <f>31991+29965</f>
-        <v>61956</v>
-      </c>
+      <c r="AW75" s="25"/>
+      <c r="AX75" s="25"/>
+      <c r="AY75" s="25"/>
+      <c r="AZ75" s="25"/>
       <c r="BA75" s="6"/>
       <c r="BB75" s="25"/>
-      <c r="BC75" s="25">
-        <f>34245+32884</f>
-        <v>67129</v>
-      </c>
-      <c r="BD75" s="25">
-        <f>33858+33125</f>
-        <v>66983</v>
-      </c>
+      <c r="BC75" s="25"/>
+      <c r="BD75" s="25"/>
       <c r="BE75" s="25"/>
       <c r="BF75" s="25"/>
       <c r="BG75" s="6"/>
@@ -11449,10 +11292,7 @@
       <c r="AR76" s="25"/>
       <c r="AS76" s="6"/>
       <c r="AT76" s="6"/>
-      <c r="AU76" s="25">
-        <f>12019.5+1042</f>
-        <v>13061.5</v>
-      </c>
+      <c r="AU76" s="25"/>
       <c r="AV76" s="25"/>
       <c r="AW76" s="25"/>
       <c r="AX76" s="25"/>
@@ -11803,24 +11643,15 @@
       <c r="AR79" s="25"/>
       <c r="AS79" s="6"/>
       <c r="AT79" s="6"/>
-      <c r="AU79" s="25">
-        <v>25160</v>
-      </c>
-      <c r="AV79" s="25">
-        <v>25087</v>
-      </c>
+      <c r="AU79" s="25"/>
+      <c r="AV79" s="25"/>
       <c r="AW79" s="25"/>
       <c r="AX79" s="25"/>
-      <c r="AY79" s="25">
-        <f>24430.6+24425.6</f>
-        <v>48856.2</v>
-      </c>
+      <c r="AY79" s="25"/>
       <c r="AZ79" s="26"/>
       <c r="BA79" s="6"/>
       <c r="BB79" s="25"/>
-      <c r="BC79" s="25">
-        <v>24482.6</v>
-      </c>
+      <c r="BC79" s="25"/>
       <c r="BD79" s="25"/>
       <c r="BE79" s="25"/>
       <c r="BF79" s="25"/>
@@ -12054,14 +11885,10 @@
       <c r="AR81" s="25"/>
       <c r="AS81" s="6"/>
       <c r="AT81" s="6"/>
-      <c r="AU81" s="25">
-        <v>22876</v>
-      </c>
+      <c r="AU81" s="25"/>
       <c r="AV81" s="25"/>
       <c r="AW81" s="25"/>
-      <c r="AX81" s="25">
-        <v>24809</v>
-      </c>
+      <c r="AX81" s="25"/>
       <c r="AY81" s="25"/>
       <c r="AZ81" s="26"/>
       <c r="BA81" s="6"/>
@@ -12275,15 +12102,11 @@
       <c r="AV83" s="25"/>
       <c r="AW83" s="25"/>
       <c r="AX83" s="25"/>
-      <c r="AY83" s="25">
-        <v>10209</v>
-      </c>
+      <c r="AY83" s="25"/>
       <c r="AZ83" s="26"/>
       <c r="BA83" s="6"/>
       <c r="BB83" s="25"/>
-      <c r="BC83" s="25">
-        <v>12551.8</v>
-      </c>
+      <c r="BC83" s="25"/>
       <c r="BD83" s="25"/>
       <c r="BE83" s="25"/>
       <c r="BF83" s="25"/>
@@ -12386,9 +12209,7 @@
       <c r="AR84" s="25"/>
       <c r="AS84" s="6"/>
       <c r="AT84" s="6"/>
-      <c r="AU84" s="25">
-        <v>574</v>
-      </c>
+      <c r="AU84" s="25"/>
       <c r="AV84" s="25"/>
       <c r="AW84" s="25"/>
       <c r="AX84" s="25"/>
@@ -12499,10 +12320,7 @@
       <c r="AR85" s="25"/>
       <c r="AS85" s="6"/>
       <c r="AT85" s="6"/>
-      <c r="AU85" s="25">
-        <f>1544+1582</f>
-        <v>3126</v>
-      </c>
+      <c r="AU85" s="25"/>
       <c r="AV85" s="25"/>
       <c r="AW85" s="25"/>
       <c r="AX85" s="25"/>
@@ -14485,9 +14303,7 @@
       <c r="AR102" s="25"/>
       <c r="AS102" s="6"/>
       <c r="AT102" s="6"/>
-      <c r="AU102" s="25">
-        <v>89.4</v>
-      </c>
+      <c r="AU102" s="25"/>
       <c r="AV102" s="25"/>
       <c r="AW102" s="25"/>
       <c r="AX102" s="25"/>
@@ -15328,9 +15144,7 @@
       <c r="AR109" s="25"/>
       <c r="AS109" s="6"/>
       <c r="AT109" s="6"/>
-      <c r="AU109" s="25">
-        <v>167.85</v>
-      </c>
+      <c r="AU109" s="25"/>
       <c r="AV109" s="25"/>
       <c r="AW109" s="25"/>
       <c r="AX109" s="25"/>
@@ -15569,9 +15383,7 @@
       <c r="AY111" s="25"/>
       <c r="AZ111" s="26"/>
       <c r="BA111" s="6"/>
-      <c r="BB111" s="25">
-        <v>6</v>
-      </c>
+      <c r="BB111" s="25"/>
       <c r="BC111" s="25"/>
       <c r="BD111" s="25"/>
       <c r="BE111" s="25"/>
@@ -15682,9 +15494,7 @@
       <c r="AY112" s="25"/>
       <c r="AZ112" s="26"/>
       <c r="BA112" s="6"/>
-      <c r="BB112" s="25">
-        <v>5</v>
-      </c>
+      <c r="BB112" s="25"/>
       <c r="BC112" s="25"/>
       <c r="BD112" s="25"/>
       <c r="BE112" s="25"/>
@@ -15795,9 +15605,7 @@
       <c r="AY113" s="25"/>
       <c r="AZ113" s="26"/>
       <c r="BA113" s="6"/>
-      <c r="BB113" s="25">
-        <v>10</v>
-      </c>
+      <c r="BB113" s="25"/>
       <c r="BC113" s="25"/>
       <c r="BD113" s="25"/>
       <c r="BE113" s="25"/>
@@ -15902,9 +15710,7 @@
       <c r="AS114" s="6"/>
       <c r="AT114" s="6"/>
       <c r="AU114" s="25"/>
-      <c r="AV114" s="25">
-        <v>15</v>
-      </c>
+      <c r="AV114" s="25"/>
       <c r="AW114" s="25"/>
       <c r="AX114" s="25"/>
       <c r="AY114" s="25"/>
@@ -16014,9 +15820,7 @@
       <c r="AR115" s="25"/>
       <c r="AS115" s="6"/>
       <c r="AT115" s="6"/>
-      <c r="AU115" s="25">
-        <v>108</v>
-      </c>
+      <c r="AU115" s="25"/>
       <c r="AV115" s="25"/>
       <c r="AW115" s="25"/>
       <c r="AX115" s="25"/>
@@ -16128,9 +15932,7 @@
       <c r="AS116" s="6"/>
       <c r="AT116" s="6"/>
       <c r="AU116" s="25"/>
-      <c r="AV116" s="25">
-        <v>3</v>
-      </c>
+      <c r="AV116" s="25"/>
       <c r="AW116" s="25"/>
       <c r="AX116" s="25"/>
       <c r="AY116" s="25"/>
@@ -16352,9 +16154,7 @@
       <c r="AS118" s="6"/>
       <c r="AT118" s="6"/>
       <c r="AU118" s="25"/>
-      <c r="AV118" s="25">
-        <v>2</v>
-      </c>
+      <c r="AV118" s="25"/>
       <c r="AW118" s="25"/>
       <c r="AX118" s="25"/>
       <c r="AY118" s="25"/>
@@ -18148,10 +17948,7 @@
       <c r="AS133" s="6"/>
       <c r="AT133" s="6"/>
       <c r="AU133" s="25"/>
-      <c r="AV133" s="25">
-        <f>5000+5760</f>
-        <v>10760</v>
-      </c>
+      <c r="AV133" s="25"/>
       <c r="AW133" s="25"/>
       <c r="AX133" s="25"/>
       <c r="AY133" s="25"/>
@@ -18272,10 +18069,7 @@
       <c r="AS134" s="6"/>
       <c r="AT134" s="6"/>
       <c r="AU134" s="25"/>
-      <c r="AV134" s="25">
-        <f>7500+5100</f>
-        <v>12600</v>
-      </c>
+      <c r="AV134" s="25"/>
       <c r="AW134" s="25"/>
       <c r="AX134" s="25"/>
       <c r="AY134" s="25"/>
@@ -18396,9 +18190,7 @@
       <c r="AS135" s="6"/>
       <c r="AT135" s="6"/>
       <c r="AU135" s="25"/>
-      <c r="AV135" s="25">
-        <v>4840</v>
-      </c>
+      <c r="AV135" s="25"/>
       <c r="AW135" s="25"/>
       <c r="AX135" s="25"/>
       <c r="AY135" s="25"/>
@@ -18519,9 +18311,7 @@
       <c r="AS136" s="6"/>
       <c r="AT136" s="6"/>
       <c r="AU136" s="25"/>
-      <c r="AV136" s="25">
-        <v>2000</v>
-      </c>
+      <c r="AV136" s="25"/>
       <c r="AW136" s="25"/>
       <c r="AX136" s="25"/>
       <c r="AY136" s="25"/>
@@ -18634,9 +18424,7 @@
       <c r="AT137" s="6"/>
       <c r="AU137" s="25"/>
       <c r="AV137" s="25"/>
-      <c r="AW137" s="25">
-        <v>75</v>
-      </c>
+      <c r="AW137" s="25"/>
       <c r="AX137" s="25"/>
       <c r="AY137" s="25"/>
       <c r="AZ137" s="26"/>
@@ -18746,26 +18534,16 @@
       <c r="AR138" s="25"/>
       <c r="AS138" s="6"/>
       <c r="AT138" s="6"/>
-      <c r="AU138" s="25">
-        <v>72</v>
-      </c>
-      <c r="AV138" s="25">
-        <v>144</v>
-      </c>
+      <c r="AU138" s="25"/>
+      <c r="AV138" s="25"/>
       <c r="AW138" s="25"/>
-      <c r="AX138" s="25">
-        <v>72</v>
-      </c>
+      <c r="AX138" s="25"/>
       <c r="AY138" s="25"/>
       <c r="AZ138" s="26"/>
       <c r="BA138" s="6"/>
-      <c r="BB138" s="25">
-        <v>72</v>
-      </c>
+      <c r="BB138" s="25"/>
       <c r="BC138" s="25"/>
-      <c r="BD138" s="25">
-        <v>72</v>
-      </c>
+      <c r="BD138" s="25"/>
       <c r="BE138" s="25"/>
       <c r="BF138" s="25"/>
       <c r="BG138" s="6"/>
@@ -18869,26 +18647,16 @@
       <c r="AR139" s="25"/>
       <c r="AS139" s="6"/>
       <c r="AT139" s="6"/>
-      <c r="AU139" s="25">
-        <v>48</v>
-      </c>
-      <c r="AV139" s="25">
-        <v>96</v>
-      </c>
+      <c r="AU139" s="25"/>
+      <c r="AV139" s="25"/>
       <c r="AW139" s="25"/>
-      <c r="AX139" s="25">
-        <v>144</v>
-      </c>
+      <c r="AX139" s="25"/>
       <c r="AY139" s="25"/>
       <c r="AZ139" s="26"/>
       <c r="BA139" s="6"/>
-      <c r="BB139" s="25">
-        <v>36</v>
-      </c>
+      <c r="BB139" s="25"/>
       <c r="BC139" s="25"/>
-      <c r="BD139" s="25">
-        <v>48</v>
-      </c>
+      <c r="BD139" s="25"/>
       <c r="BE139" s="25"/>
       <c r="BF139" s="25"/>
       <c r="BG139" s="6"/>
@@ -18996,21 +18764,14 @@
       <c r="AR140" s="25"/>
       <c r="AS140" s="6"/>
       <c r="AT140" s="6"/>
-      <c r="AU140" s="25">
-        <f>192+36</f>
-        <v>228</v>
-      </c>
+      <c r="AU140" s="25"/>
       <c r="AV140" s="25"/>
-      <c r="AW140" s="25">
-        <v>36</v>
-      </c>
+      <c r="AW140" s="25"/>
       <c r="AX140" s="25"/>
       <c r="AY140" s="25"/>
       <c r="AZ140" s="26"/>
       <c r="BA140" s="6"/>
-      <c r="BB140" s="25">
-        <v>96</v>
-      </c>
+      <c r="BB140" s="25"/>
       <c r="BC140" s="25"/>
       <c r="BD140" s="25"/>
       <c r="BE140" s="25"/>
@@ -19102,23 +18863,16 @@
       <c r="AR141" s="25"/>
       <c r="AS141" s="6"/>
       <c r="AT141" s="6"/>
-      <c r="AU141" s="25">
-        <v>40</v>
-      </c>
+      <c r="AU141" s="25"/>
       <c r="AV141" s="25"/>
       <c r="AW141" s="25"/>
-      <c r="AX141" s="25">
-        <f>40+40</f>
-        <v>80</v>
-      </c>
+      <c r="AX141" s="25"/>
       <c r="AY141" s="25"/>
       <c r="AZ141" s="26"/>
       <c r="BA141" s="6"/>
       <c r="BB141" s="25"/>
       <c r="BC141" s="25"/>
-      <c r="BD141" s="25">
-        <v>40</v>
-      </c>
+      <c r="BD141" s="25"/>
       <c r="BE141" s="25"/>
       <c r="BF141" s="25"/>
       <c r="BG141" s="6"/>
@@ -19220,9 +18974,7 @@
       <c r="AT142" s="6"/>
       <c r="AU142" s="25"/>
       <c r="AV142" s="25"/>
-      <c r="AW142" s="25">
-        <v>75</v>
-      </c>
+      <c r="AW142" s="25"/>
       <c r="AX142" s="25"/>
       <c r="AY142" s="25"/>
       <c r="AZ142" s="26"/>
@@ -19334,9 +19086,7 @@
       <c r="AS143" s="6"/>
       <c r="AT143" s="6"/>
       <c r="AU143" s="25"/>
-      <c r="AV143" s="25">
-        <v>72</v>
-      </c>
+      <c r="AV143" s="25"/>
       <c r="AW143" s="25"/>
       <c r="AX143" s="25"/>
       <c r="AY143" s="25"/>
@@ -19449,12 +19199,8 @@
       <c r="AS144" s="6"/>
       <c r="AT144" s="6"/>
       <c r="AU144" s="25"/>
-      <c r="AV144" s="25">
-        <v>48</v>
-      </c>
-      <c r="AW144" s="25">
-        <v>48</v>
-      </c>
+      <c r="AV144" s="25"/>
+      <c r="AW144" s="25"/>
       <c r="AX144" s="25"/>
       <c r="AY144" s="25"/>
       <c r="AZ144" s="26"/>
@@ -19566,12 +19312,8 @@
       <c r="AS145" s="6"/>
       <c r="AT145" s="6"/>
       <c r="AU145" s="25"/>
-      <c r="AV145" s="25">
-        <v>72</v>
-      </c>
-      <c r="AW145" s="25">
-        <v>36</v>
-      </c>
+      <c r="AV145" s="25"/>
+      <c r="AW145" s="25"/>
       <c r="AX145" s="25"/>
       <c r="AY145" s="25"/>
       <c r="AZ145" s="26"/>
@@ -19903,20 +19645,14 @@
       <c r="AR148" s="25"/>
       <c r="AS148" s="6"/>
       <c r="AT148" s="6"/>
-      <c r="AU148" s="25">
-        <v>133</v>
-      </c>
+      <c r="AU148" s="25"/>
       <c r="AV148" s="25"/>
       <c r="AW148" s="25"/>
-      <c r="AX148" s="25">
-        <v>98</v>
-      </c>
+      <c r="AX148" s="25"/>
       <c r="AY148" s="25"/>
       <c r="AZ148" s="26"/>
       <c r="BA148" s="6"/>
-      <c r="BB148" s="25">
-        <v>154</v>
-      </c>
+      <c r="BB148" s="25"/>
       <c r="BC148" s="25"/>
       <c r="BD148" s="25"/>
       <c r="BE148" s="25"/>
@@ -20020,22 +19756,14 @@
       <c r="AR149" s="25"/>
       <c r="AS149" s="6"/>
       <c r="AT149" s="6"/>
-      <c r="AU149" s="25">
-        <v>99</v>
-      </c>
-      <c r="AV149" s="25">
-        <v>108</v>
-      </c>
+      <c r="AU149" s="25"/>
+      <c r="AV149" s="25"/>
       <c r="AW149" s="25"/>
-      <c r="AX149" s="25">
-        <v>90</v>
-      </c>
+      <c r="AX149" s="25"/>
       <c r="AY149" s="25"/>
       <c r="AZ149" s="26"/>
       <c r="BA149" s="6"/>
-      <c r="BB149" s="25">
-        <v>108</v>
-      </c>
+      <c r="BB149" s="25"/>
       <c r="BC149" s="25"/>
       <c r="BD149" s="25"/>
       <c r="BE149" s="25"/>
@@ -20243,9 +19971,7 @@
       <c r="AR151" s="25"/>
       <c r="AS151" s="6"/>
       <c r="AT151" s="6"/>
-      <c r="AU151" s="25">
-        <v>42</v>
-      </c>
+      <c r="AU151" s="25"/>
       <c r="AV151" s="25"/>
       <c r="AW151" s="25"/>
       <c r="AX151" s="25"/>
@@ -20474,15 +20200,11 @@
       <c r="AU153" s="25"/>
       <c r="AV153" s="25"/>
       <c r="AW153" s="25"/>
-      <c r="AX153" s="25">
-        <v>49</v>
-      </c>
+      <c r="AX153" s="25"/>
       <c r="AY153" s="25"/>
       <c r="AZ153" s="26"/>
       <c r="BA153" s="6"/>
-      <c r="BB153" s="25">
-        <v>49</v>
-      </c>
+      <c r="BB153" s="25"/>
       <c r="BC153" s="25"/>
       <c r="BD153" s="25"/>
       <c r="BE153" s="25"/>
@@ -20588,9 +20310,7 @@
       <c r="AU154" s="25"/>
       <c r="AV154" s="25"/>
       <c r="AW154" s="25"/>
-      <c r="AX154" s="25">
-        <v>99</v>
-      </c>
+      <c r="AX154" s="25"/>
       <c r="AY154" s="25"/>
       <c r="AZ154" s="26"/>
       <c r="BA154" s="6"/>
@@ -20693,15 +20413,11 @@
       <c r="AU155" s="25"/>
       <c r="AV155" s="25"/>
       <c r="AW155" s="25"/>
-      <c r="AX155" s="25">
-        <v>35</v>
-      </c>
+      <c r="AX155" s="25"/>
       <c r="AY155" s="25"/>
       <c r="AZ155" s="26"/>
       <c r="BA155" s="6"/>
-      <c r="BB155" s="25">
-        <v>42</v>
-      </c>
+      <c r="BB155" s="25"/>
       <c r="BC155" s="25"/>
       <c r="BD155" s="25"/>
       <c r="BE155" s="25"/>
@@ -20810,9 +20526,7 @@
       <c r="AW156" s="25"/>
       <c r="AX156" s="25"/>
       <c r="AY156" s="25"/>
-      <c r="AZ156" s="25">
-        <v>20</v>
-      </c>
+      <c r="AZ156" s="25"/>
       <c r="BA156" s="6"/>
       <c r="BB156" s="25"/>
       <c r="BC156" s="25"/>
@@ -20921,20 +20635,14 @@
       <c r="AR157" s="25"/>
       <c r="AS157" s="6"/>
       <c r="AT157" s="6"/>
-      <c r="AU157" s="25">
-        <v>14</v>
-      </c>
+      <c r="AU157" s="25"/>
       <c r="AV157" s="25"/>
       <c r="AW157" s="25"/>
-      <c r="AX157" s="25">
-        <v>14</v>
-      </c>
+      <c r="AX157" s="25"/>
       <c r="AY157" s="25"/>
       <c r="AZ157" s="26"/>
       <c r="BA157" s="6"/>
-      <c r="BB157" s="25">
-        <v>14</v>
-      </c>
+      <c r="BB157" s="25"/>
       <c r="BC157" s="25"/>
       <c r="BD157" s="25"/>
       <c r="BE157" s="25"/>
@@ -21892,9 +21600,7 @@
       <c r="AT166" s="6"/>
       <c r="AU166" s="25"/>
       <c r="AV166" s="25"/>
-      <c r="AW166" s="25">
-        <v>200</v>
-      </c>
+      <c r="AW166" s="25"/>
       <c r="AX166" s="25"/>
       <c r="AY166" s="25"/>
       <c r="AZ166" s="26"/>
@@ -21985,9 +21691,7 @@
       <c r="AT167" s="6"/>
       <c r="AU167" s="25"/>
       <c r="AV167" s="25"/>
-      <c r="AW167" s="25">
-        <v>600</v>
-      </c>
+      <c r="AW167" s="25"/>
       <c r="AX167" s="25"/>
       <c r="AY167" s="25"/>
       <c r="AZ167" s="26"/>
@@ -22107,9 +21811,7 @@
       <c r="AT168" s="6"/>
       <c r="AU168" s="25"/>
       <c r="AV168" s="25"/>
-      <c r="AW168" s="25">
-        <v>600</v>
-      </c>
+      <c r="AW168" s="25"/>
       <c r="AX168" s="25"/>
       <c r="AY168" s="25"/>
       <c r="AZ168" s="26"/>
@@ -22332,20 +22034,14 @@
       <c r="AT170" s="6"/>
       <c r="AU170" s="25"/>
       <c r="AV170" s="25"/>
-      <c r="AW170" s="25">
-        <v>9000</v>
-      </c>
+      <c r="AW170" s="25"/>
       <c r="AX170" s="25"/>
       <c r="AY170" s="25"/>
-      <c r="AZ170" s="25">
-        <v>1500</v>
-      </c>
+      <c r="AZ170" s="25"/>
       <c r="BA170" s="6"/>
       <c r="BB170" s="25"/>
       <c r="BC170" s="25"/>
-      <c r="BD170" s="25">
-        <v>1500</v>
-      </c>
+      <c r="BD170" s="25"/>
       <c r="BE170" s="25"/>
       <c r="BF170" s="25"/>
       <c r="BG170" s="6"/>
@@ -22447,22 +22143,16 @@
       <c r="AR171" s="25"/>
       <c r="AS171" s="6"/>
       <c r="AT171" s="6"/>
-      <c r="AU171" s="25">
-        <v>5000</v>
-      </c>
+      <c r="AU171" s="25"/>
       <c r="AV171" s="25"/>
-      <c r="AW171" s="25">
-        <v>16000</v>
-      </c>
+      <c r="AW171" s="25"/>
       <c r="AX171" s="25"/>
       <c r="AY171" s="25"/>
       <c r="AZ171" s="26"/>
       <c r="BA171" s="6"/>
       <c r="BB171" s="25"/>
       <c r="BC171" s="25"/>
-      <c r="BD171" s="25">
-        <v>1000</v>
-      </c>
+      <c r="BD171" s="25"/>
       <c r="BE171" s="25"/>
       <c r="BF171" s="25"/>
       <c r="BG171" s="6"/>
@@ -22566,20 +22256,14 @@
       <c r="AT172" s="6"/>
       <c r="AU172" s="25"/>
       <c r="AV172" s="25"/>
-      <c r="AW172" s="25">
-        <v>10000</v>
-      </c>
+      <c r="AW172" s="25"/>
       <c r="AX172" s="25"/>
       <c r="AY172" s="25"/>
-      <c r="AZ172" s="25">
-        <v>2000</v>
-      </c>
+      <c r="AZ172" s="25"/>
       <c r="BA172" s="6"/>
       <c r="BB172" s="25"/>
       <c r="BC172" s="25"/>
-      <c r="BD172" s="25">
-        <v>3000</v>
-      </c>
+      <c r="BD172" s="25"/>
       <c r="BE172" s="25"/>
       <c r="BF172" s="25"/>
       <c r="BG172" s="6"/>
@@ -22684,20 +22368,14 @@
       <c r="AT173" s="6"/>
       <c r="AU173" s="25"/>
       <c r="AV173" s="25"/>
-      <c r="AW173" s="25">
-        <v>3000</v>
-      </c>
+      <c r="AW173" s="25"/>
       <c r="AX173" s="25"/>
       <c r="AY173" s="25"/>
-      <c r="AZ173" s="25">
-        <v>1000</v>
-      </c>
+      <c r="AZ173" s="25"/>
       <c r="BA173" s="6"/>
       <c r="BB173" s="25"/>
       <c r="BC173" s="25"/>
-      <c r="BD173" s="25">
-        <v>3000</v>
-      </c>
+      <c r="BD173" s="25"/>
       <c r="BE173" s="25"/>
       <c r="BF173" s="25"/>
       <c r="BG173" s="6"/>
@@ -22914,9 +22592,7 @@
       <c r="AS175" s="6"/>
       <c r="AT175" s="6"/>
       <c r="AU175" s="25"/>
-      <c r="AV175" s="25">
-        <v>3000</v>
-      </c>
+      <c r="AV175" s="25"/>
       <c r="AW175" s="25"/>
       <c r="AX175" s="25"/>
       <c r="AY175" s="25"/>
@@ -23032,9 +22708,7 @@
       <c r="AS176" s="6"/>
       <c r="AT176" s="6"/>
       <c r="AU176" s="25"/>
-      <c r="AV176" s="25">
-        <v>3000</v>
-      </c>
+      <c r="AV176" s="25"/>
       <c r="AW176" s="25"/>
       <c r="AX176" s="25"/>
       <c r="AY176" s="25"/>
@@ -23150,9 +22824,7 @@
       <c r="AS177" s="6"/>
       <c r="AT177" s="6"/>
       <c r="AU177" s="25"/>
-      <c r="AV177" s="25">
-        <v>2000</v>
-      </c>
+      <c r="AV177" s="25"/>
       <c r="AW177" s="25"/>
       <c r="AX177" s="25"/>
       <c r="AY177" s="25"/>
@@ -23271,9 +22943,7 @@
       <c r="AS178" s="6"/>
       <c r="AT178" s="6"/>
       <c r="AU178" s="25"/>
-      <c r="AV178" s="25">
-        <v>1000</v>
-      </c>
+      <c r="AV178" s="25"/>
       <c r="AW178" s="25"/>
       <c r="AX178" s="25"/>
       <c r="AY178" s="25"/>
@@ -23501,17 +23171,13 @@
       <c r="AU180" s="25"/>
       <c r="AV180" s="25"/>
       <c r="AW180" s="25"/>
-      <c r="AX180" s="25">
-        <v>2000</v>
-      </c>
+      <c r="AX180" s="25"/>
       <c r="AY180" s="25"/>
       <c r="AZ180" s="26"/>
       <c r="BA180" s="6"/>
       <c r="BB180" s="25"/>
       <c r="BC180" s="25"/>
-      <c r="BD180" s="25">
-        <v>2000</v>
-      </c>
+      <c r="BD180" s="25"/>
       <c r="BE180" s="25"/>
       <c r="BF180" s="25"/>
       <c r="BG180" s="6"/>
@@ -23709,17 +23375,13 @@
       <c r="AU182" s="25"/>
       <c r="AV182" s="25"/>
       <c r="AW182" s="25"/>
-      <c r="AX182" s="25">
-        <v>2500</v>
-      </c>
+      <c r="AX182" s="25"/>
       <c r="AY182" s="25"/>
       <c r="AZ182" s="26"/>
       <c r="BA182" s="6"/>
       <c r="BB182" s="25"/>
       <c r="BC182" s="25"/>
-      <c r="BD182" s="25">
-        <v>2500</v>
-      </c>
+      <c r="BD182" s="25"/>
       <c r="BE182" s="25"/>
       <c r="BF182" s="25"/>
       <c r="BG182" s="6"/>
@@ -23820,9 +23482,7 @@
       <c r="AU183" s="25"/>
       <c r="AV183" s="25"/>
       <c r="AW183" s="25"/>
-      <c r="AX183" s="25">
-        <v>3600</v>
-      </c>
+      <c r="AX183" s="25"/>
       <c r="AY183" s="25"/>
       <c r="AZ183" s="26"/>
       <c r="BA183" s="6"/>
@@ -24041,9 +23701,7 @@
       <c r="AS185" s="6"/>
       <c r="AT185" s="6"/>
       <c r="AU185" s="25"/>
-      <c r="AV185" s="25">
-        <v>30</v>
-      </c>
+      <c r="AV185" s="25"/>
       <c r="AW185" s="25"/>
       <c r="AX185" s="25"/>
       <c r="AY185" s="25"/>
@@ -24051,9 +23709,7 @@
       <c r="BA185" s="6"/>
       <c r="BB185" s="25"/>
       <c r="BC185" s="25"/>
-      <c r="BD185" s="25">
-        <v>25</v>
-      </c>
+      <c r="BD185" s="25"/>
       <c r="BE185" s="25"/>
       <c r="BF185" s="25"/>
       <c r="BG185" s="6"/>
@@ -24274,9 +23930,7 @@
       <c r="AV187" s="25"/>
       <c r="AW187" s="25"/>
       <c r="AX187" s="25"/>
-      <c r="AY187" s="25">
-        <v>250</v>
-      </c>
+      <c r="AY187" s="25"/>
       <c r="AZ187" s="26"/>
       <c r="BA187" s="6"/>
       <c r="BB187" s="25"/>
@@ -24499,9 +24153,7 @@
       <c r="BA189" s="6"/>
       <c r="BB189" s="25"/>
       <c r="BC189" s="25"/>
-      <c r="BD189" s="25">
-        <v>80</v>
-      </c>
+      <c r="BD189" s="25"/>
       <c r="BE189" s="25"/>
       <c r="BF189" s="25"/>
       <c r="BG189" s="6"/>
@@ -24717,9 +24369,7 @@
       <c r="AU191" s="25"/>
       <c r="AV191" s="25"/>
       <c r="AW191" s="25"/>
-      <c r="AX191" s="25">
-        <v>80</v>
-      </c>
+      <c r="AX191" s="25"/>
       <c r="AY191" s="25"/>
       <c r="AZ191" s="26"/>
       <c r="BA191" s="6"/>
@@ -24829,12 +24479,8 @@
       <c r="AT192" s="6"/>
       <c r="AU192" s="25"/>
       <c r="AV192" s="25"/>
-      <c r="AW192" s="25">
-        <v>50</v>
-      </c>
-      <c r="AX192" s="25">
-        <v>102</v>
-      </c>
+      <c r="AW192" s="25"/>
+      <c r="AX192" s="25"/>
       <c r="AY192" s="25"/>
       <c r="AZ192" s="26"/>
       <c r="BA192" s="6"/>
@@ -24945,9 +24591,7 @@
       <c r="AU193" s="25"/>
       <c r="AV193" s="25"/>
       <c r="AW193" s="25"/>
-      <c r="AX193" s="25">
-        <v>45</v>
-      </c>
+      <c r="AX193" s="25"/>
       <c r="AY193" s="25"/>
       <c r="AZ193" s="26"/>
       <c r="BA193" s="6"/>
@@ -25171,9 +24815,7 @@
       <c r="AV195" s="25"/>
       <c r="AW195" s="25"/>
       <c r="AX195" s="25"/>
-      <c r="AY195" s="25">
-        <v>48</v>
-      </c>
+      <c r="AY195" s="25"/>
       <c r="AZ195" s="26"/>
       <c r="BA195" s="6"/>
       <c r="BB195" s="25"/>
@@ -25522,10 +25164,7 @@
       <c r="AR198" s="25"/>
       <c r="AS198" s="6"/>
       <c r="AT198" s="6"/>
-      <c r="AU198" s="25">
-        <f>500+500</f>
-        <v>1000</v>
-      </c>
+      <c r="AU198" s="25"/>
       <c r="AV198" s="25"/>
       <c r="AW198" s="25"/>
       <c r="AX198" s="25"/>
@@ -26354,9 +25993,7 @@
       <c r="AU205" s="25"/>
       <c r="AV205" s="25"/>
       <c r="AW205" s="25"/>
-      <c r="AX205" s="25">
-        <v>500</v>
-      </c>
+      <c r="AX205" s="25"/>
       <c r="AY205" s="25"/>
       <c r="AZ205" s="26"/>
       <c r="BA205" s="6"/>
@@ -26470,9 +26107,7 @@
       <c r="AY206" s="25"/>
       <c r="AZ206" s="26"/>
       <c r="BA206" s="6"/>
-      <c r="BB206" s="25">
-        <v>296</v>
-      </c>
+      <c r="BB206" s="25"/>
       <c r="BC206" s="25"/>
       <c r="BD206" s="25"/>
       <c r="BE206" s="25"/>
@@ -26584,9 +26219,7 @@
       <c r="AY207" s="25"/>
       <c r="AZ207" s="26"/>
       <c r="BA207" s="6"/>
-      <c r="BB207" s="25">
-        <v>296</v>
-      </c>
+      <c r="BB207" s="25"/>
       <c r="BC207" s="25"/>
       <c r="BD207" s="25"/>
       <c r="BE207" s="25"/>
@@ -27827,9 +27460,7 @@
       <c r="AY218" s="25"/>
       <c r="AZ218" s="26"/>
       <c r="BA218" s="6"/>
-      <c r="BB218" s="25">
-        <v>42</v>
-      </c>
+      <c r="BB218" s="25"/>
       <c r="BC218" s="25"/>
       <c r="BD218" s="25"/>
       <c r="BE218" s="25"/>
@@ -28158,9 +27789,7 @@
       <c r="AU221" s="25"/>
       <c r="AV221" s="25"/>
       <c r="AW221" s="25"/>
-      <c r="AX221" s="25">
-        <v>40</v>
-      </c>
+      <c r="AX221" s="25"/>
       <c r="AY221" s="25"/>
       <c r="AZ221" s="26"/>
       <c r="BA221" s="6"/>
@@ -29935,9 +29564,7 @@
       <c r="AR237" s="25"/>
       <c r="AS237" s="6"/>
       <c r="AT237" s="6"/>
-      <c r="AU237" s="25">
-        <v>300</v>
-      </c>
+      <c r="AU237" s="25"/>
       <c r="AV237" s="25"/>
       <c r="AW237" s="25"/>
       <c r="AX237" s="25"/>
@@ -32371,474 +31998,435 @@
   </sheetData>
   <autoFilter ref="C2:D2" xr:uid="{CC412B54-366C-48C5-A561-3550BE0946A4}"/>
   <conditionalFormatting sqref="F38">
-    <cfRule type="cellIs" dxfId="118" priority="381" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="108" priority="381" operator="lessThanOrEqual">
       <formula>$G38</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="378" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="378" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="379" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="106" priority="379" operator="greaterThanOrEqual">
       <formula>$H38</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="380" operator="between">
+    <cfRule type="cellIs" dxfId="105" priority="380" operator="between">
       <formula>$G38</formula>
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24">
-    <cfRule type="cellIs" dxfId="114" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="156" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="155" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="103" priority="155" operator="lessThanOrEqual">
       <formula>$F24</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="154" operator="between">
+    <cfRule type="cellIs" dxfId="102" priority="154" operator="between">
       <formula>$F24</formula>
       <formula>$H24</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="153" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="101" priority="153" operator="greaterThanOrEqual">
       <formula>$G24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J65">
-    <cfRule type="cellIs" dxfId="110" priority="173" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="100" priority="173" operator="greaterThanOrEqual">
       <formula>$F65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="174" operator="between">
+    <cfRule type="cellIs" dxfId="99" priority="174" operator="between">
       <formula>$E65</formula>
       <formula>$G65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="175" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="98" priority="175" operator="lessThanOrEqual">
       <formula>$E65</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J66:J67 J70 M70:Q70 J99 M99:Q99 J203 M203:Q203">
-    <cfRule type="cellIs" dxfId="107" priority="178" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="97" priority="178" operator="lessThanOrEqual">
       <formula>$G66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="177" operator="between">
+    <cfRule type="cellIs" dxfId="96" priority="177" operator="between">
       <formula>$G66</formula>
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="176" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="95" priority="176" operator="greaterThanOrEqual">
       <formula>$H66</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J76">
-    <cfRule type="cellIs" dxfId="104" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="157" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J108 J130 M130:Q130 J132 M132:Q132">
-    <cfRule type="cellIs" dxfId="103" priority="163" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="93" priority="163" operator="lessThanOrEqual">
       <formula>$F108</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="162" operator="between">
+    <cfRule type="cellIs" dxfId="92" priority="162" operator="between">
       <formula>$F108</formula>
       <formula>$H108</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="161" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="91" priority="161" operator="greaterThanOrEqual">
       <formula>$G108</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J125">
-    <cfRule type="cellIs" dxfId="100" priority="168" operator="between">
+    <cfRule type="cellIs" dxfId="90" priority="168" operator="between">
       <formula>$F125</formula>
       <formula>$H125</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="167" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="89" priority="167" operator="greaterThanOrEqual">
       <formula>$G125</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="169" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="88" priority="169" operator="lessThanOrEqual">
       <formula>$F125</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J134">
-    <cfRule type="cellIs" dxfId="97" priority="172" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="87" priority="172" operator="lessThanOrEqual">
       <formula>$F134</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="171" operator="between">
+    <cfRule type="cellIs" dxfId="86" priority="171" operator="between">
       <formula>$F134</formula>
       <formula>$H134</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="170" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="85" priority="170" operator="greaterThanOrEqual">
       <formula>$G134</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J151:J152">
-    <cfRule type="cellIs" dxfId="94" priority="152" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="84" priority="152" operator="lessThanOrEqual">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="151" operator="between">
+    <cfRule type="cellIs" dxfId="83" priority="151" operator="between">
       <formula>#REF!</formula>
       <formula>$F151</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="150" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="82" priority="150" operator="greaterThanOrEqual">
       <formula>$E151</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="149" operator="equal">
       <formula>$F$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J163:J164">
-    <cfRule type="cellIs" dxfId="90" priority="148" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="80" priority="148" operator="lessThanOrEqual">
       <formula>$F163</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="147" operator="between">
+    <cfRule type="cellIs" dxfId="79" priority="147" operator="between">
       <formula>$F163</formula>
       <formula>$H163</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="146" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="78" priority="146" operator="greaterThanOrEqual">
       <formula>$G163</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J217">
-    <cfRule type="cellIs" dxfId="87" priority="166" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="77" priority="166" operator="lessThanOrEqual">
       <formula>$F217</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="164" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="76" priority="164" operator="greaterThanOrEqual">
       <formula>$G217</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="165" operator="between">
+    <cfRule type="cellIs" dxfId="75" priority="165" operator="between">
       <formula>$F217</formula>
       <formula>$H217</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J236">
-    <cfRule type="cellIs" dxfId="84" priority="158" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="74" priority="158" operator="greaterThanOrEqual">
       <formula>$G236</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="159" operator="between">
+    <cfRule type="cellIs" dxfId="73" priority="159" operator="between">
       <formula>$F236</formula>
       <formula>$H236</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="160" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="72" priority="160" operator="lessThanOrEqual">
       <formula>$F236</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M24:Q24">
-    <cfRule type="cellIs" dxfId="81" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="123" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="120" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="70" priority="120" operator="greaterThanOrEqual">
       <formula>$G24</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="121" operator="between">
+    <cfRule type="cellIs" dxfId="69" priority="121" operator="between">
       <formula>$F24</formula>
       <formula>$H24</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="122" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="68" priority="122" operator="lessThanOrEqual">
       <formula>$F24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M65:Q65">
-    <cfRule type="cellIs" dxfId="77" priority="141" operator="between">
+    <cfRule type="cellIs" dxfId="67" priority="141" operator="between">
       <formula>$E65</formula>
       <formula>$G65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="142" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="66" priority="142" operator="lessThanOrEqual">
       <formula>$E65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="140" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="65" priority="140" operator="greaterThanOrEqual">
       <formula>$F65</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M66:Q67">
-    <cfRule type="cellIs" dxfId="74" priority="78" operator="between">
+    <cfRule type="cellIs" dxfId="64" priority="78" operator="between">
       <formula>$G66</formula>
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="79" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="63" priority="79" operator="lessThanOrEqual">
       <formula>$G66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="77" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="62" priority="77" operator="greaterThanOrEqual">
       <formula>$H66</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M76:Q76">
-    <cfRule type="cellIs" dxfId="71" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="124" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M108:Q108">
-    <cfRule type="cellIs" dxfId="70" priority="130" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="60" priority="130" operator="lessThanOrEqual">
       <formula>$F108</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="129" operator="between">
+    <cfRule type="cellIs" dxfId="59" priority="129" operator="between">
       <formula>$F108</formula>
       <formula>$H108</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="128" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="58" priority="128" operator="greaterThanOrEqual">
       <formula>$G108</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M125:Q125">
-    <cfRule type="cellIs" dxfId="67" priority="135" operator="between">
+    <cfRule type="cellIs" dxfId="57" priority="135" operator="between">
       <formula>$F125</formula>
       <formula>$H125</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="134" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="56" priority="134" operator="greaterThanOrEqual">
       <formula>$G125</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="136" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="55" priority="136" operator="lessThanOrEqual">
       <formula>$F125</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M134:Q134">
-    <cfRule type="cellIs" dxfId="64" priority="138" operator="between">
+    <cfRule type="cellIs" dxfId="54" priority="138" operator="between">
       <formula>$F134</formula>
       <formula>$H134</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="139" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="53" priority="139" operator="lessThanOrEqual">
       <formula>$F134</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="137" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="52" priority="137" operator="greaterThanOrEqual">
       <formula>$G134</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M151:Q152">
-    <cfRule type="cellIs" dxfId="61" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="73" operator="equal">
       <formula>$F$1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="74" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="50" priority="74" operator="greaterThanOrEqual">
       <formula>$E151</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="75" operator="between">
+    <cfRule type="cellIs" dxfId="49" priority="75" operator="between">
       <formula>#REF!</formula>
       <formula>$F151</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="76" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="48" priority="76" operator="lessThanOrEqual">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M163:Q164">
-    <cfRule type="cellIs" dxfId="57" priority="70" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="47" priority="70" operator="greaterThanOrEqual">
       <formula>$G163</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="71" operator="between">
+    <cfRule type="cellIs" dxfId="46" priority="71" operator="between">
       <formula>$F163</formula>
       <formula>$H163</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="72" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="45" priority="72" operator="lessThanOrEqual">
       <formula>$F163</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M217:Q217">
-    <cfRule type="cellIs" dxfId="54" priority="131" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="44" priority="131" operator="greaterThanOrEqual">
       <formula>$G217</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="132" operator="between">
+    <cfRule type="cellIs" dxfId="43" priority="132" operator="between">
       <formula>$F217</formula>
       <formula>$H217</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="133" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="42" priority="133" operator="lessThanOrEqual">
       <formula>$F217</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M236:Q236">
-    <cfRule type="cellIs" dxfId="51" priority="125" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="41" priority="125" operator="greaterThanOrEqual">
       <formula>$G236</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="127" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="40" priority="127" operator="lessThanOrEqual">
       <formula>$F236</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="126" operator="between">
+    <cfRule type="cellIs" dxfId="39" priority="126" operator="between">
       <formula>$F236</formula>
       <formula>$H236</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T24:W24">
-    <cfRule type="cellIs" dxfId="48" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="44" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="43" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="37" priority="43" operator="lessThanOrEqual">
       <formula>$F24</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="41" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="36" priority="41" operator="greaterThanOrEqual">
       <formula>$G24</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="42" operator="between">
+    <cfRule type="cellIs" dxfId="35" priority="42" operator="between">
       <formula>$F24</formula>
       <formula>$H24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T65:W65">
-    <cfRule type="cellIs" dxfId="44" priority="61" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="34" priority="61" operator="greaterThanOrEqual">
       <formula>$F65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="63" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="33" priority="63" operator="lessThanOrEqual">
       <formula>$E65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="62" operator="between">
+    <cfRule type="cellIs" dxfId="32" priority="62" operator="between">
       <formula>$E65</formula>
       <formula>$G65</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T66:V67">
-    <cfRule type="cellIs" dxfId="41" priority="18" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="T66:W67">
+    <cfRule type="cellIs" dxfId="31" priority="8" operator="greaterThanOrEqual">
       <formula>$H66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="19" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="9" operator="between">
       <formula>$G66</formula>
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="20" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="29" priority="10" operator="lessThanOrEqual">
       <formula>$G66</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T70:W70 T99:W99 T203:W203">
-    <cfRule type="cellIs" dxfId="38" priority="67" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="28" priority="67" operator="greaterThanOrEqual">
       <formula>$H70</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="69" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="27" priority="69" operator="lessThanOrEqual">
       <formula>$G70</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="68" operator="between">
+    <cfRule type="cellIs" dxfId="26" priority="68" operator="between">
       <formula>$G70</formula>
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T76:W76">
-    <cfRule type="cellIs" dxfId="35" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="45" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T108:W108">
-    <cfRule type="cellIs" dxfId="34" priority="49" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="49" operator="greaterThanOrEqual">
       <formula>$G108</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="51" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="23" priority="51" operator="lessThanOrEqual">
       <formula>$F108</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="50" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="50" operator="between">
       <formula>$F108</formula>
       <formula>$H108</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T125:W125">
-    <cfRule type="cellIs" dxfId="31" priority="57" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="21" priority="57" operator="lessThanOrEqual">
       <formula>$F125</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="55" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="20" priority="55" operator="greaterThanOrEqual">
       <formula>$G125</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="56" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="56" operator="between">
       <formula>$F125</formula>
       <formula>$H125</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T130:W130 T132:W132">
-    <cfRule type="cellIs" dxfId="28" priority="65" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="65" operator="between">
       <formula>$F130</formula>
       <formula>$H130</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="66" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="17" priority="66" operator="lessThanOrEqual">
       <formula>$F130</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="64" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="64" operator="greaterThanOrEqual">
       <formula>$G130</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T134:W134">
-    <cfRule type="cellIs" dxfId="25" priority="58" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="15" priority="58" operator="greaterThanOrEqual">
       <formula>$G134</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="59" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="59" operator="between">
       <formula>$F134</formula>
       <formula>$H134</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="60" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="60" operator="lessThanOrEqual">
       <formula>$F134</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T151:V152">
-    <cfRule type="cellIs" dxfId="22" priority="17" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="T151:W152">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="lessThanOrEqual">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="16" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="between">
       <formula>#REF!</formula>
       <formula>$F151</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="greaterThanOrEqual">
       <formula>$E151</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>$F$1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T163:V164">
-    <cfRule type="cellIs" dxfId="18" priority="13" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="T163:W164">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="lessThanOrEqual">
       <formula>$F163</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThanOrEqual">
       <formula>$G163</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="between">
       <formula>$F163</formula>
       <formula>$H163</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T217:W217">
-    <cfRule type="cellIs" dxfId="15" priority="52" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="52" operator="greaterThanOrEqual">
       <formula>$G217</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="53" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="53" operator="between">
       <formula>$F217</formula>
       <formula>$H217</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="54" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="54" operator="lessThanOrEqual">
       <formula>$F217</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T236:W236">
-    <cfRule type="cellIs" dxfId="12" priority="46" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="46" operator="greaterThanOrEqual">
       <formula>$G236</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="47" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="47" operator="between">
       <formula>$F236</formula>
       <formula>$H236</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="48" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="48" operator="lessThanOrEqual">
       <formula>$F236</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W66:W67">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="greaterThanOrEqual">
-      <formula>$H66</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="between">
-      <formula>$G66</formula>
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="lessThanOrEqual">
-      <formula>$G66</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W151:W152">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>$F$1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThanOrEqual">
-      <formula>$E151</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="between">
-      <formula>#REF!</formula>
-      <formula>$F151</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThanOrEqual">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W163:W164">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
-      <formula>$G163</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="between">
-      <formula>$F163</formula>
-      <formula>$H163</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThanOrEqual">
-      <formula>$F163</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
:test_tube: test:Testando funcionalidades para a página 'Demanda por polimeros'
</commit_message>
<xml_diff>
--- a/script/.database/Novembro-2024.xlsx
+++ b/script/.database/Novembro-2024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Almoxarifado suprimentos\Suprimentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\PCP\CLAUDIO\VS_CD\dash\DashBoard_cd\script\.database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B6AA41-01BE-4BAF-BB33-E6E95D911C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2196D0-398C-44F4-ACCC-D8661799C58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{206D94FF-8DD9-460F-9052-07E07C6EA2D8}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{206D94FF-8DD9-460F-9052-07E07C6EA2D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -1148,77 +1148,7 @@
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
     <cellStyle name="Vírgula 2 3" xfId="2" xr:uid="{D464673A-692A-4B68-AAA0-4458BA1E072D}"/>
   </cellStyles>
-  <dxfs count="119">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="109">
     <dxf>
       <fill>
         <patternFill>
@@ -2322,11 +2252,11 @@
   <dimension ref="A1:WZG553"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
-      <selection pane="bottomRight" activeCell="W3" sqref="W3"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -2336,8 +2266,8 @@
     <col min="4" max="4" width="70.85546875" style="46" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" style="47" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" style="27" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="10.7109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="27" bestFit="1" customWidth="1"/>
     <col min="10" max="39" width="9.42578125" style="27" customWidth="1"/>
     <col min="40" max="40" width="15.7109375" style="27" customWidth="1"/>
     <col min="41" max="41" width="12.42578125" style="1" customWidth="1"/>
@@ -2868,16 +2798,11 @@
       <c r="AR3" s="25"/>
       <c r="AS3" s="6"/>
       <c r="AT3" s="6"/>
-      <c r="AU3" s="25">
-        <v>12500</v>
-      </c>
+      <c r="AU3" s="25"/>
       <c r="AV3" s="25"/>
       <c r="AW3" s="25"/>
       <c r="AX3" s="25"/>
-      <c r="AY3" s="25">
-        <f>12500+12500</f>
-        <v>25000</v>
-      </c>
+      <c r="AY3" s="25"/>
       <c r="AZ3" s="26"/>
       <c r="BA3" s="6"/>
       <c r="BB3" s="25"/>
@@ -3351,9 +3276,7 @@
       <c r="AZ7" s="26"/>
       <c r="BA7" s="6"/>
       <c r="BB7" s="25"/>
-      <c r="BC7" s="25">
-        <v>1250</v>
-      </c>
+      <c r="BC7" s="25"/>
       <c r="BD7" s="25"/>
       <c r="BE7" s="25"/>
       <c r="BF7" s="25"/>
@@ -3587,9 +3510,7 @@
       <c r="AR9" s="25"/>
       <c r="AS9" s="6"/>
       <c r="AT9" s="6"/>
-      <c r="AU9" s="25">
-        <v>500</v>
-      </c>
+      <c r="AU9" s="25"/>
       <c r="AV9" s="25"/>
       <c r="AW9" s="25"/>
       <c r="AX9" s="25"/>
@@ -3710,9 +3631,7 @@
       <c r="AR10" s="25"/>
       <c r="AS10" s="6"/>
       <c r="AT10" s="6"/>
-      <c r="AU10" s="25">
-        <v>500</v>
-      </c>
+      <c r="AU10" s="25"/>
       <c r="AV10" s="25"/>
       <c r="AW10" s="25"/>
       <c r="AX10" s="25"/>
@@ -3833,9 +3752,7 @@
       <c r="AR11" s="25"/>
       <c r="AS11" s="6"/>
       <c r="AT11" s="6"/>
-      <c r="AU11" s="25">
-        <v>400</v>
-      </c>
+      <c r="AU11" s="25"/>
       <c r="AV11" s="25"/>
       <c r="AW11" s="25"/>
       <c r="AX11" s="25"/>
@@ -3956,9 +3873,7 @@
       <c r="AR12" s="25"/>
       <c r="AS12" s="6"/>
       <c r="AT12" s="6"/>
-      <c r="AU12" s="25">
-        <v>200</v>
-      </c>
+      <c r="AU12" s="25"/>
       <c r="AV12" s="25"/>
       <c r="AW12" s="25"/>
       <c r="AX12" s="25"/>
@@ -4079,9 +3994,7 @@
       <c r="AR13" s="25"/>
       <c r="AS13" s="6"/>
       <c r="AT13" s="6"/>
-      <c r="AU13" s="25">
-        <v>200</v>
-      </c>
+      <c r="AU13" s="25"/>
       <c r="AV13" s="25"/>
       <c r="AW13" s="25"/>
       <c r="AX13" s="25"/>
@@ -4089,9 +4002,7 @@
       <c r="AZ13" s="26"/>
       <c r="BA13" s="6"/>
       <c r="BB13" s="25"/>
-      <c r="BC13" s="25">
-        <v>300</v>
-      </c>
+      <c r="BC13" s="25"/>
       <c r="BD13" s="25"/>
       <c r="BE13" s="25"/>
       <c r="BF13" s="25"/>
@@ -4213,9 +4124,7 @@
       <c r="AZ14" s="26"/>
       <c r="BA14" s="6"/>
       <c r="BB14" s="25"/>
-      <c r="BC14" s="25">
-        <v>300</v>
-      </c>
+      <c r="BC14" s="25"/>
       <c r="BD14" s="25"/>
       <c r="BE14" s="25"/>
       <c r="BF14" s="25"/>
@@ -4440,20 +4349,14 @@
       <c r="AS16" s="6"/>
       <c r="AT16" s="6"/>
       <c r="AU16" s="25"/>
-      <c r="AV16" s="25">
-        <v>12000</v>
-      </c>
+      <c r="AV16" s="25"/>
       <c r="AW16" s="25"/>
       <c r="AX16" s="25"/>
-      <c r="AY16" s="25">
-        <v>12000</v>
-      </c>
+      <c r="AY16" s="25"/>
       <c r="AZ16" s="26"/>
       <c r="BA16" s="6"/>
       <c r="BB16" s="25"/>
-      <c r="BC16" s="25">
-        <v>12600</v>
-      </c>
+      <c r="BC16" s="25"/>
       <c r="BD16" s="25"/>
       <c r="BE16" s="25"/>
       <c r="BF16" s="25"/>
@@ -4910,9 +4813,7 @@
       <c r="AV20" s="25"/>
       <c r="AW20" s="25"/>
       <c r="AX20" s="25"/>
-      <c r="AY20" s="25">
-        <v>5000</v>
-      </c>
+      <c r="AY20" s="25"/>
       <c r="AZ20" s="26"/>
       <c r="BA20" s="6"/>
       <c r="BB20" s="25"/>
@@ -5030,9 +4931,7 @@
       <c r="AY21" s="25"/>
       <c r="AZ21" s="26"/>
       <c r="BA21" s="6"/>
-      <c r="BB21" s="25">
-        <v>1250</v>
-      </c>
+      <c r="BB21" s="25"/>
       <c r="BC21" s="25"/>
       <c r="BD21" s="25"/>
       <c r="BE21" s="25"/>
@@ -5268,9 +5167,7 @@
       <c r="AU23" s="25"/>
       <c r="AV23" s="25"/>
       <c r="AW23" s="25"/>
-      <c r="AX23" s="25">
-        <v>6300</v>
-      </c>
+      <c r="AX23" s="25"/>
       <c r="AY23" s="25"/>
       <c r="AZ23" s="26"/>
       <c r="BA23" s="6"/>
@@ -5504,10 +5401,7 @@
       <c r="BA25" s="6"/>
       <c r="BB25" s="25"/>
       <c r="BC25" s="25"/>
-      <c r="BD25" s="25">
-        <f>15000+15000</f>
-        <v>30000</v>
-      </c>
+      <c r="BD25" s="25"/>
       <c r="BE25" s="25"/>
       <c r="BF25" s="25"/>
       <c r="BG25" s="6"/>
@@ -5981,9 +5875,7 @@
       <c r="AS29" s="6"/>
       <c r="AT29" s="6"/>
       <c r="AU29" s="25"/>
-      <c r="AV29" s="25">
-        <v>12600</v>
-      </c>
+      <c r="AV29" s="25"/>
       <c r="AW29" s="25"/>
       <c r="AX29" s="25"/>
       <c r="AY29" s="25"/>
@@ -5991,9 +5883,7 @@
       <c r="BA29" s="6"/>
       <c r="BB29" s="25"/>
       <c r="BC29" s="25"/>
-      <c r="BD29" s="25">
-        <v>15000</v>
-      </c>
+      <c r="BD29" s="25"/>
       <c r="BE29" s="25"/>
       <c r="BF29" s="25"/>
       <c r="BG29" s="6"/>
@@ -6105,20 +5995,14 @@
       <c r="AR30" s="25"/>
       <c r="AS30" s="6"/>
       <c r="AT30" s="6"/>
-      <c r="AU30" s="25">
-        <v>12600</v>
-      </c>
+      <c r="AU30" s="25"/>
       <c r="AV30" s="25"/>
       <c r="AW30" s="25"/>
-      <c r="AX30" s="25">
-        <v>12600</v>
-      </c>
+      <c r="AX30" s="25"/>
       <c r="AY30" s="25"/>
       <c r="AZ30" s="26"/>
       <c r="BA30" s="6"/>
-      <c r="BB30" s="25">
-        <v>12600</v>
-      </c>
+      <c r="BB30" s="25"/>
       <c r="BC30" s="25"/>
       <c r="BD30" s="25"/>
       <c r="BE30" s="25"/>
@@ -6231,21 +6115,15 @@
       <c r="AS31" s="6"/>
       <c r="AT31" s="6"/>
       <c r="AU31" s="25"/>
-      <c r="AV31" s="25">
-        <v>12600</v>
-      </c>
+      <c r="AV31" s="25"/>
       <c r="AW31" s="25"/>
       <c r="AX31" s="25"/>
-      <c r="AY31" s="25">
-        <v>12600</v>
-      </c>
+      <c r="AY31" s="25"/>
       <c r="AZ31" s="26"/>
       <c r="BA31" s="6"/>
       <c r="BB31" s="25"/>
       <c r="BC31" s="25"/>
-      <c r="BD31" s="25">
-        <v>12600</v>
-      </c>
+      <c r="BD31" s="25"/>
       <c r="BE31" s="25"/>
       <c r="BF31" s="25"/>
       <c r="BG31" s="6"/>
@@ -6358,15 +6236,11 @@
       <c r="AS32" s="6"/>
       <c r="AT32" s="6"/>
       <c r="AU32" s="25"/>
-      <c r="AV32" s="25">
-        <v>12600</v>
-      </c>
+      <c r="AV32" s="25"/>
       <c r="AW32" s="25"/>
       <c r="AX32" s="25"/>
       <c r="AY32" s="25"/>
-      <c r="AZ32" s="25">
-        <v>12500</v>
-      </c>
+      <c r="AZ32" s="25"/>
       <c r="BA32" s="6"/>
       <c r="BB32" s="25"/>
       <c r="BC32" s="25"/>
@@ -6954,19 +6828,13 @@
       <c r="AU37" s="25"/>
       <c r="AV37" s="25"/>
       <c r="AW37" s="25"/>
-      <c r="AX37" s="25">
-        <v>1000</v>
-      </c>
+      <c r="AX37" s="25"/>
       <c r="AY37" s="25"/>
       <c r="AZ37" s="26"/>
       <c r="BA37" s="6"/>
       <c r="BB37" s="25"/>
-      <c r="BC37" s="25">
-        <v>1000</v>
-      </c>
-      <c r="BD37" s="25">
-        <v>1000</v>
-      </c>
+      <c r="BC37" s="25"/>
+      <c r="BD37" s="25"/>
       <c r="BE37" s="25"/>
       <c r="BF37" s="25"/>
       <c r="BG37" s="6"/>
@@ -7206,9 +7074,7 @@
       <c r="BA39" s="6"/>
       <c r="BB39" s="25"/>
       <c r="BC39" s="25"/>
-      <c r="BD39" s="25">
-        <v>150</v>
-      </c>
+      <c r="BD39" s="25"/>
       <c r="BE39" s="25"/>
       <c r="BF39" s="25"/>
       <c r="BG39" s="6"/>
@@ -7444,9 +7310,7 @@
       <c r="BA41" s="6"/>
       <c r="BB41" s="25"/>
       <c r="BC41" s="25"/>
-      <c r="BD41" s="25">
-        <v>150</v>
-      </c>
+      <c r="BD41" s="25"/>
       <c r="BE41" s="25"/>
       <c r="BF41" s="25"/>
       <c r="BG41" s="6"/>
@@ -10859,9 +10723,7 @@
       <c r="AU71" s="25"/>
       <c r="AV71" s="25"/>
       <c r="AW71" s="25"/>
-      <c r="AX71" s="25">
-        <v>301.95</v>
-      </c>
+      <c r="AX71" s="25"/>
       <c r="AY71" s="25"/>
       <c r="AZ71" s="26"/>
       <c r="BA71" s="6"/>
@@ -11322,38 +11184,19 @@
       <c r="AO75" s="24"/>
       <c r="AP75" s="24"/>
       <c r="AQ75" s="24"/>
-      <c r="AR75" s="25">
-        <v>25014</v>
-      </c>
+      <c r="AR75" s="25"/>
       <c r="AS75" s="6"/>
       <c r="AT75" s="6"/>
       <c r="AU75" s="25"/>
       <c r="AV75" s="25"/>
-      <c r="AW75" s="25">
-        <v>29672</v>
-      </c>
-      <c r="AX75" s="25">
-        <f>34022+32942</f>
-        <v>66964</v>
-      </c>
-      <c r="AY75" s="25">
-        <f>34199+33913</f>
-        <v>68112</v>
-      </c>
-      <c r="AZ75" s="25">
-        <f>31991+29965</f>
-        <v>61956</v>
-      </c>
+      <c r="AW75" s="25"/>
+      <c r="AX75" s="25"/>
+      <c r="AY75" s="25"/>
+      <c r="AZ75" s="25"/>
       <c r="BA75" s="6"/>
       <c r="BB75" s="25"/>
-      <c r="BC75" s="25">
-        <f>34245+32884</f>
-        <v>67129</v>
-      </c>
-      <c r="BD75" s="25">
-        <f>33858+33125</f>
-        <v>66983</v>
-      </c>
+      <c r="BC75" s="25"/>
+      <c r="BD75" s="25"/>
       <c r="BE75" s="25"/>
       <c r="BF75" s="25"/>
       <c r="BG75" s="6"/>
@@ -11449,10 +11292,7 @@
       <c r="AR76" s="25"/>
       <c r="AS76" s="6"/>
       <c r="AT76" s="6"/>
-      <c r="AU76" s="25">
-        <f>12019.5+1042</f>
-        <v>13061.5</v>
-      </c>
+      <c r="AU76" s="25"/>
       <c r="AV76" s="25"/>
       <c r="AW76" s="25"/>
       <c r="AX76" s="25"/>
@@ -11803,24 +11643,15 @@
       <c r="AR79" s="25"/>
       <c r="AS79" s="6"/>
       <c r="AT79" s="6"/>
-      <c r="AU79" s="25">
-        <v>25160</v>
-      </c>
-      <c r="AV79" s="25">
-        <v>25087</v>
-      </c>
+      <c r="AU79" s="25"/>
+      <c r="AV79" s="25"/>
       <c r="AW79" s="25"/>
       <c r="AX79" s="25"/>
-      <c r="AY79" s="25">
-        <f>24430.6+24425.6</f>
-        <v>48856.2</v>
-      </c>
+      <c r="AY79" s="25"/>
       <c r="AZ79" s="26"/>
       <c r="BA79" s="6"/>
       <c r="BB79" s="25"/>
-      <c r="BC79" s="25">
-        <v>24482.6</v>
-      </c>
+      <c r="BC79" s="25"/>
       <c r="BD79" s="25"/>
       <c r="BE79" s="25"/>
       <c r="BF79" s="25"/>
@@ -12054,14 +11885,10 @@
       <c r="AR81" s="25"/>
       <c r="AS81" s="6"/>
       <c r="AT81" s="6"/>
-      <c r="AU81" s="25">
-        <v>22876</v>
-      </c>
+      <c r="AU81" s="25"/>
       <c r="AV81" s="25"/>
       <c r="AW81" s="25"/>
-      <c r="AX81" s="25">
-        <v>24809</v>
-      </c>
+      <c r="AX81" s="25"/>
       <c r="AY81" s="25"/>
       <c r="AZ81" s="26"/>
       <c r="BA81" s="6"/>
@@ -12275,15 +12102,11 @@
       <c r="AV83" s="25"/>
       <c r="AW83" s="25"/>
       <c r="AX83" s="25"/>
-      <c r="AY83" s="25">
-        <v>10209</v>
-      </c>
+      <c r="AY83" s="25"/>
       <c r="AZ83" s="26"/>
       <c r="BA83" s="6"/>
       <c r="BB83" s="25"/>
-      <c r="BC83" s="25">
-        <v>12551.8</v>
-      </c>
+      <c r="BC83" s="25"/>
       <c r="BD83" s="25"/>
       <c r="BE83" s="25"/>
       <c r="BF83" s="25"/>
@@ -12386,9 +12209,7 @@
       <c r="AR84" s="25"/>
       <c r="AS84" s="6"/>
       <c r="AT84" s="6"/>
-      <c r="AU84" s="25">
-        <v>574</v>
-      </c>
+      <c r="AU84" s="25"/>
       <c r="AV84" s="25"/>
       <c r="AW84" s="25"/>
       <c r="AX84" s="25"/>
@@ -12499,10 +12320,7 @@
       <c r="AR85" s="25"/>
       <c r="AS85" s="6"/>
       <c r="AT85" s="6"/>
-      <c r="AU85" s="25">
-        <f>1544+1582</f>
-        <v>3126</v>
-      </c>
+      <c r="AU85" s="25"/>
       <c r="AV85" s="25"/>
       <c r="AW85" s="25"/>
       <c r="AX85" s="25"/>
@@ -14485,9 +14303,7 @@
       <c r="AR102" s="25"/>
       <c r="AS102" s="6"/>
       <c r="AT102" s="6"/>
-      <c r="AU102" s="25">
-        <v>89.4</v>
-      </c>
+      <c r="AU102" s="25"/>
       <c r="AV102" s="25"/>
       <c r="AW102" s="25"/>
       <c r="AX102" s="25"/>
@@ -15328,9 +15144,7 @@
       <c r="AR109" s="25"/>
       <c r="AS109" s="6"/>
       <c r="AT109" s="6"/>
-      <c r="AU109" s="25">
-        <v>167.85</v>
-      </c>
+      <c r="AU109" s="25"/>
       <c r="AV109" s="25"/>
       <c r="AW109" s="25"/>
       <c r="AX109" s="25"/>
@@ -15569,9 +15383,7 @@
       <c r="AY111" s="25"/>
       <c r="AZ111" s="26"/>
       <c r="BA111" s="6"/>
-      <c r="BB111" s="25">
-        <v>6</v>
-      </c>
+      <c r="BB111" s="25"/>
       <c r="BC111" s="25"/>
       <c r="BD111" s="25"/>
       <c r="BE111" s="25"/>
@@ -15682,9 +15494,7 @@
       <c r="AY112" s="25"/>
       <c r="AZ112" s="26"/>
       <c r="BA112" s="6"/>
-      <c r="BB112" s="25">
-        <v>5</v>
-      </c>
+      <c r="BB112" s="25"/>
       <c r="BC112" s="25"/>
       <c r="BD112" s="25"/>
       <c r="BE112" s="25"/>
@@ -15795,9 +15605,7 @@
       <c r="AY113" s="25"/>
       <c r="AZ113" s="26"/>
       <c r="BA113" s="6"/>
-      <c r="BB113" s="25">
-        <v>10</v>
-      </c>
+      <c r="BB113" s="25"/>
       <c r="BC113" s="25"/>
       <c r="BD113" s="25"/>
       <c r="BE113" s="25"/>
@@ -15902,9 +15710,7 @@
       <c r="AS114" s="6"/>
       <c r="AT114" s="6"/>
       <c r="AU114" s="25"/>
-      <c r="AV114" s="25">
-        <v>15</v>
-      </c>
+      <c r="AV114" s="25"/>
       <c r="AW114" s="25"/>
       <c r="AX114" s="25"/>
       <c r="AY114" s="25"/>
@@ -16014,9 +15820,7 @@
       <c r="AR115" s="25"/>
       <c r="AS115" s="6"/>
       <c r="AT115" s="6"/>
-      <c r="AU115" s="25">
-        <v>108</v>
-      </c>
+      <c r="AU115" s="25"/>
       <c r="AV115" s="25"/>
       <c r="AW115" s="25"/>
       <c r="AX115" s="25"/>
@@ -16128,9 +15932,7 @@
       <c r="AS116" s="6"/>
       <c r="AT116" s="6"/>
       <c r="AU116" s="25"/>
-      <c r="AV116" s="25">
-        <v>3</v>
-      </c>
+      <c r="AV116" s="25"/>
       <c r="AW116" s="25"/>
       <c r="AX116" s="25"/>
       <c r="AY116" s="25"/>
@@ -16352,9 +16154,7 @@
       <c r="AS118" s="6"/>
       <c r="AT118" s="6"/>
       <c r="AU118" s="25"/>
-      <c r="AV118" s="25">
-        <v>2</v>
-      </c>
+      <c r="AV118" s="25"/>
       <c r="AW118" s="25"/>
       <c r="AX118" s="25"/>
       <c r="AY118" s="25"/>
@@ -18148,10 +17948,7 @@
       <c r="AS133" s="6"/>
       <c r="AT133" s="6"/>
       <c r="AU133" s="25"/>
-      <c r="AV133" s="25">
-        <f>5000+5760</f>
-        <v>10760</v>
-      </c>
+      <c r="AV133" s="25"/>
       <c r="AW133" s="25"/>
       <c r="AX133" s="25"/>
       <c r="AY133" s="25"/>
@@ -18272,10 +18069,7 @@
       <c r="AS134" s="6"/>
       <c r="AT134" s="6"/>
       <c r="AU134" s="25"/>
-      <c r="AV134" s="25">
-        <f>7500+5100</f>
-        <v>12600</v>
-      </c>
+      <c r="AV134" s="25"/>
       <c r="AW134" s="25"/>
       <c r="AX134" s="25"/>
       <c r="AY134" s="25"/>
@@ -18396,9 +18190,7 @@
       <c r="AS135" s="6"/>
       <c r="AT135" s="6"/>
       <c r="AU135" s="25"/>
-      <c r="AV135" s="25">
-        <v>4840</v>
-      </c>
+      <c r="AV135" s="25"/>
       <c r="AW135" s="25"/>
       <c r="AX135" s="25"/>
       <c r="AY135" s="25"/>
@@ -18519,9 +18311,7 @@
       <c r="AS136" s="6"/>
       <c r="AT136" s="6"/>
       <c r="AU136" s="25"/>
-      <c r="AV136" s="25">
-        <v>2000</v>
-      </c>
+      <c r="AV136" s="25"/>
       <c r="AW136" s="25"/>
       <c r="AX136" s="25"/>
       <c r="AY136" s="25"/>
@@ -18634,9 +18424,7 @@
       <c r="AT137" s="6"/>
       <c r="AU137" s="25"/>
       <c r="AV137" s="25"/>
-      <c r="AW137" s="25">
-        <v>75</v>
-      </c>
+      <c r="AW137" s="25"/>
       <c r="AX137" s="25"/>
       <c r="AY137" s="25"/>
       <c r="AZ137" s="26"/>
@@ -18746,26 +18534,16 @@
       <c r="AR138" s="25"/>
       <c r="AS138" s="6"/>
       <c r="AT138" s="6"/>
-      <c r="AU138" s="25">
-        <v>72</v>
-      </c>
-      <c r="AV138" s="25">
-        <v>144</v>
-      </c>
+      <c r="AU138" s="25"/>
+      <c r="AV138" s="25"/>
       <c r="AW138" s="25"/>
-      <c r="AX138" s="25">
-        <v>72</v>
-      </c>
+      <c r="AX138" s="25"/>
       <c r="AY138" s="25"/>
       <c r="AZ138" s="26"/>
       <c r="BA138" s="6"/>
-      <c r="BB138" s="25">
-        <v>72</v>
-      </c>
+      <c r="BB138" s="25"/>
       <c r="BC138" s="25"/>
-      <c r="BD138" s="25">
-        <v>72</v>
-      </c>
+      <c r="BD138" s="25"/>
       <c r="BE138" s="25"/>
       <c r="BF138" s="25"/>
       <c r="BG138" s="6"/>
@@ -18869,26 +18647,16 @@
       <c r="AR139" s="25"/>
       <c r="AS139" s="6"/>
       <c r="AT139" s="6"/>
-      <c r="AU139" s="25">
-        <v>48</v>
-      </c>
-      <c r="AV139" s="25">
-        <v>96</v>
-      </c>
+      <c r="AU139" s="25"/>
+      <c r="AV139" s="25"/>
       <c r="AW139" s="25"/>
-      <c r="AX139" s="25">
-        <v>144</v>
-      </c>
+      <c r="AX139" s="25"/>
       <c r="AY139" s="25"/>
       <c r="AZ139" s="26"/>
       <c r="BA139" s="6"/>
-      <c r="BB139" s="25">
-        <v>36</v>
-      </c>
+      <c r="BB139" s="25"/>
       <c r="BC139" s="25"/>
-      <c r="BD139" s="25">
-        <v>48</v>
-      </c>
+      <c r="BD139" s="25"/>
       <c r="BE139" s="25"/>
       <c r="BF139" s="25"/>
       <c r="BG139" s="6"/>
@@ -18996,21 +18764,14 @@
       <c r="AR140" s="25"/>
       <c r="AS140" s="6"/>
       <c r="AT140" s="6"/>
-      <c r="AU140" s="25">
-        <f>192+36</f>
-        <v>228</v>
-      </c>
+      <c r="AU140" s="25"/>
       <c r="AV140" s="25"/>
-      <c r="AW140" s="25">
-        <v>36</v>
-      </c>
+      <c r="AW140" s="25"/>
       <c r="AX140" s="25"/>
       <c r="AY140" s="25"/>
       <c r="AZ140" s="26"/>
       <c r="BA140" s="6"/>
-      <c r="BB140" s="25">
-        <v>96</v>
-      </c>
+      <c r="BB140" s="25"/>
       <c r="BC140" s="25"/>
       <c r="BD140" s="25"/>
       <c r="BE140" s="25"/>
@@ -19102,23 +18863,16 @@
       <c r="AR141" s="25"/>
       <c r="AS141" s="6"/>
       <c r="AT141" s="6"/>
-      <c r="AU141" s="25">
-        <v>40</v>
-      </c>
+      <c r="AU141" s="25"/>
       <c r="AV141" s="25"/>
       <c r="AW141" s="25"/>
-      <c r="AX141" s="25">
-        <f>40+40</f>
-        <v>80</v>
-      </c>
+      <c r="AX141" s="25"/>
       <c r="AY141" s="25"/>
       <c r="AZ141" s="26"/>
       <c r="BA141" s="6"/>
       <c r="BB141" s="25"/>
       <c r="BC141" s="25"/>
-      <c r="BD141" s="25">
-        <v>40</v>
-      </c>
+      <c r="BD141" s="25"/>
       <c r="BE141" s="25"/>
       <c r="BF141" s="25"/>
       <c r="BG141" s="6"/>
@@ -19220,9 +18974,7 @@
       <c r="AT142" s="6"/>
       <c r="AU142" s="25"/>
       <c r="AV142" s="25"/>
-      <c r="AW142" s="25">
-        <v>75</v>
-      </c>
+      <c r="AW142" s="25"/>
       <c r="AX142" s="25"/>
       <c r="AY142" s="25"/>
       <c r="AZ142" s="26"/>
@@ -19334,9 +19086,7 @@
       <c r="AS143" s="6"/>
       <c r="AT143" s="6"/>
       <c r="AU143" s="25"/>
-      <c r="AV143" s="25">
-        <v>72</v>
-      </c>
+      <c r="AV143" s="25"/>
       <c r="AW143" s="25"/>
       <c r="AX143" s="25"/>
       <c r="AY143" s="25"/>
@@ -19449,12 +19199,8 @@
       <c r="AS144" s="6"/>
       <c r="AT144" s="6"/>
       <c r="AU144" s="25"/>
-      <c r="AV144" s="25">
-        <v>48</v>
-      </c>
-      <c r="AW144" s="25">
-        <v>48</v>
-      </c>
+      <c r="AV144" s="25"/>
+      <c r="AW144" s="25"/>
       <c r="AX144" s="25"/>
       <c r="AY144" s="25"/>
       <c r="AZ144" s="26"/>
@@ -19566,12 +19312,8 @@
       <c r="AS145" s="6"/>
       <c r="AT145" s="6"/>
       <c r="AU145" s="25"/>
-      <c r="AV145" s="25">
-        <v>72</v>
-      </c>
-      <c r="AW145" s="25">
-        <v>36</v>
-      </c>
+      <c r="AV145" s="25"/>
+      <c r="AW145" s="25"/>
       <c r="AX145" s="25"/>
       <c r="AY145" s="25"/>
       <c r="AZ145" s="26"/>
@@ -19903,20 +19645,14 @@
       <c r="AR148" s="25"/>
       <c r="AS148" s="6"/>
       <c r="AT148" s="6"/>
-      <c r="AU148" s="25">
-        <v>133</v>
-      </c>
+      <c r="AU148" s="25"/>
       <c r="AV148" s="25"/>
       <c r="AW148" s="25"/>
-      <c r="AX148" s="25">
-        <v>98</v>
-      </c>
+      <c r="AX148" s="25"/>
       <c r="AY148" s="25"/>
       <c r="AZ148" s="26"/>
       <c r="BA148" s="6"/>
-      <c r="BB148" s="25">
-        <v>154</v>
-      </c>
+      <c r="BB148" s="25"/>
       <c r="BC148" s="25"/>
       <c r="BD148" s="25"/>
       <c r="BE148" s="25"/>
@@ -20020,22 +19756,14 @@
       <c r="AR149" s="25"/>
       <c r="AS149" s="6"/>
       <c r="AT149" s="6"/>
-      <c r="AU149" s="25">
-        <v>99</v>
-      </c>
-      <c r="AV149" s="25">
-        <v>108</v>
-      </c>
+      <c r="AU149" s="25"/>
+      <c r="AV149" s="25"/>
       <c r="AW149" s="25"/>
-      <c r="AX149" s="25">
-        <v>90</v>
-      </c>
+      <c r="AX149" s="25"/>
       <c r="AY149" s="25"/>
       <c r="AZ149" s="26"/>
       <c r="BA149" s="6"/>
-      <c r="BB149" s="25">
-        <v>108</v>
-      </c>
+      <c r="BB149" s="25"/>
       <c r="BC149" s="25"/>
       <c r="BD149" s="25"/>
       <c r="BE149" s="25"/>
@@ -20243,9 +19971,7 @@
       <c r="AR151" s="25"/>
       <c r="AS151" s="6"/>
       <c r="AT151" s="6"/>
-      <c r="AU151" s="25">
-        <v>42</v>
-      </c>
+      <c r="AU151" s="25"/>
       <c r="AV151" s="25"/>
       <c r="AW151" s="25"/>
       <c r="AX151" s="25"/>
@@ -20474,15 +20200,11 @@
       <c r="AU153" s="25"/>
       <c r="AV153" s="25"/>
       <c r="AW153" s="25"/>
-      <c r="AX153" s="25">
-        <v>49</v>
-      </c>
+      <c r="AX153" s="25"/>
       <c r="AY153" s="25"/>
       <c r="AZ153" s="26"/>
       <c r="BA153" s="6"/>
-      <c r="BB153" s="25">
-        <v>49</v>
-      </c>
+      <c r="BB153" s="25"/>
       <c r="BC153" s="25"/>
       <c r="BD153" s="25"/>
       <c r="BE153" s="25"/>
@@ -20588,9 +20310,7 @@
       <c r="AU154" s="25"/>
       <c r="AV154" s="25"/>
       <c r="AW154" s="25"/>
-      <c r="AX154" s="25">
-        <v>99</v>
-      </c>
+      <c r="AX154" s="25"/>
       <c r="AY154" s="25"/>
       <c r="AZ154" s="26"/>
       <c r="BA154" s="6"/>
@@ -20693,15 +20413,11 @@
       <c r="AU155" s="25"/>
       <c r="AV155" s="25"/>
       <c r="AW155" s="25"/>
-      <c r="AX155" s="25">
-        <v>35</v>
-      </c>
+      <c r="AX155" s="25"/>
       <c r="AY155" s="25"/>
       <c r="AZ155" s="26"/>
       <c r="BA155" s="6"/>
-      <c r="BB155" s="25">
-        <v>42</v>
-      </c>
+      <c r="BB155" s="25"/>
       <c r="BC155" s="25"/>
       <c r="BD155" s="25"/>
       <c r="BE155" s="25"/>
@@ -20810,9 +20526,7 @@
       <c r="AW156" s="25"/>
       <c r="AX156" s="25"/>
       <c r="AY156" s="25"/>
-      <c r="AZ156" s="25">
-        <v>20</v>
-      </c>
+      <c r="AZ156" s="25"/>
       <c r="BA156" s="6"/>
       <c r="BB156" s="25"/>
       <c r="BC156" s="25"/>
@@ -20921,20 +20635,14 @@
       <c r="AR157" s="25"/>
       <c r="AS157" s="6"/>
       <c r="AT157" s="6"/>
-      <c r="AU157" s="25">
-        <v>14</v>
-      </c>
+      <c r="AU157" s="25"/>
       <c r="AV157" s="25"/>
       <c r="AW157" s="25"/>
-      <c r="AX157" s="25">
-        <v>14</v>
-      </c>
+      <c r="AX157" s="25"/>
       <c r="AY157" s="25"/>
       <c r="AZ157" s="26"/>
       <c r="BA157" s="6"/>
-      <c r="BB157" s="25">
-        <v>14</v>
-      </c>
+      <c r="BB157" s="25"/>
       <c r="BC157" s="25"/>
       <c r="BD157" s="25"/>
       <c r="BE157" s="25"/>
@@ -21892,9 +21600,7 @@
       <c r="AT166" s="6"/>
       <c r="AU166" s="25"/>
       <c r="AV166" s="25"/>
-      <c r="AW166" s="25">
-        <v>200</v>
-      </c>
+      <c r="AW166" s="25"/>
       <c r="AX166" s="25"/>
       <c r="AY166" s="25"/>
       <c r="AZ166" s="26"/>
@@ -21985,9 +21691,7 @@
       <c r="AT167" s="6"/>
       <c r="AU167" s="25"/>
       <c r="AV167" s="25"/>
-      <c r="AW167" s="25">
-        <v>600</v>
-      </c>
+      <c r="AW167" s="25"/>
       <c r="AX167" s="25"/>
       <c r="AY167" s="25"/>
       <c r="AZ167" s="26"/>
@@ -22107,9 +21811,7 @@
       <c r="AT168" s="6"/>
       <c r="AU168" s="25"/>
       <c r="AV168" s="25"/>
-      <c r="AW168" s="25">
-        <v>600</v>
-      </c>
+      <c r="AW168" s="25"/>
       <c r="AX168" s="25"/>
       <c r="AY168" s="25"/>
       <c r="AZ168" s="26"/>
@@ -22332,20 +22034,14 @@
       <c r="AT170" s="6"/>
       <c r="AU170" s="25"/>
       <c r="AV170" s="25"/>
-      <c r="AW170" s="25">
-        <v>9000</v>
-      </c>
+      <c r="AW170" s="25"/>
       <c r="AX170" s="25"/>
       <c r="AY170" s="25"/>
-      <c r="AZ170" s="25">
-        <v>1500</v>
-      </c>
+      <c r="AZ170" s="25"/>
       <c r="BA170" s="6"/>
       <c r="BB170" s="25"/>
       <c r="BC170" s="25"/>
-      <c r="BD170" s="25">
-        <v>1500</v>
-      </c>
+      <c r="BD170" s="25"/>
       <c r="BE170" s="25"/>
       <c r="BF170" s="25"/>
       <c r="BG170" s="6"/>
@@ -22447,22 +22143,16 @@
       <c r="AR171" s="25"/>
       <c r="AS171" s="6"/>
       <c r="AT171" s="6"/>
-      <c r="AU171" s="25">
-        <v>5000</v>
-      </c>
+      <c r="AU171" s="25"/>
       <c r="AV171" s="25"/>
-      <c r="AW171" s="25">
-        <v>16000</v>
-      </c>
+      <c r="AW171" s="25"/>
       <c r="AX171" s="25"/>
       <c r="AY171" s="25"/>
       <c r="AZ171" s="26"/>
       <c r="BA171" s="6"/>
       <c r="BB171" s="25"/>
       <c r="BC171" s="25"/>
-      <c r="BD171" s="25">
-        <v>1000</v>
-      </c>
+      <c r="BD171" s="25"/>
       <c r="BE171" s="25"/>
       <c r="BF171" s="25"/>
       <c r="BG171" s="6"/>
@@ -22566,20 +22256,14 @@
       <c r="AT172" s="6"/>
       <c r="AU172" s="25"/>
       <c r="AV172" s="25"/>
-      <c r="AW172" s="25">
-        <v>10000</v>
-      </c>
+      <c r="AW172" s="25"/>
       <c r="AX172" s="25"/>
       <c r="AY172" s="25"/>
-      <c r="AZ172" s="25">
-        <v>2000</v>
-      </c>
+      <c r="AZ172" s="25"/>
       <c r="BA172" s="6"/>
       <c r="BB172" s="25"/>
       <c r="BC172" s="25"/>
-      <c r="BD172" s="25">
-        <v>3000</v>
-      </c>
+      <c r="BD172" s="25"/>
       <c r="BE172" s="25"/>
       <c r="BF172" s="25"/>
       <c r="BG172" s="6"/>
@@ -22684,20 +22368,14 @@
       <c r="AT173" s="6"/>
       <c r="AU173" s="25"/>
       <c r="AV173" s="25"/>
-      <c r="AW173" s="25">
-        <v>3000</v>
-      </c>
+      <c r="AW173" s="25"/>
       <c r="AX173" s="25"/>
       <c r="AY173" s="25"/>
-      <c r="AZ173" s="25">
-        <v>1000</v>
-      </c>
+      <c r="AZ173" s="25"/>
       <c r="BA173" s="6"/>
       <c r="BB173" s="25"/>
       <c r="BC173" s="25"/>
-      <c r="BD173" s="25">
-        <v>3000</v>
-      </c>
+      <c r="BD173" s="25"/>
       <c r="BE173" s="25"/>
       <c r="BF173" s="25"/>
       <c r="BG173" s="6"/>
@@ -22914,9 +22592,7 @@
       <c r="AS175" s="6"/>
       <c r="AT175" s="6"/>
       <c r="AU175" s="25"/>
-      <c r="AV175" s="25">
-        <v>3000</v>
-      </c>
+      <c r="AV175" s="25"/>
       <c r="AW175" s="25"/>
       <c r="AX175" s="25"/>
       <c r="AY175" s="25"/>
@@ -23032,9 +22708,7 @@
       <c r="AS176" s="6"/>
       <c r="AT176" s="6"/>
       <c r="AU176" s="25"/>
-      <c r="AV176" s="25">
-        <v>3000</v>
-      </c>
+      <c r="AV176" s="25"/>
       <c r="AW176" s="25"/>
       <c r="AX176" s="25"/>
       <c r="AY176" s="25"/>
@@ -23150,9 +22824,7 @@
       <c r="AS177" s="6"/>
       <c r="AT177" s="6"/>
       <c r="AU177" s="25"/>
-      <c r="AV177" s="25">
-        <v>2000</v>
-      </c>
+      <c r="AV177" s="25"/>
       <c r="AW177" s="25"/>
       <c r="AX177" s="25"/>
       <c r="AY177" s="25"/>
@@ -23271,9 +22943,7 @@
       <c r="AS178" s="6"/>
       <c r="AT178" s="6"/>
       <c r="AU178" s="25"/>
-      <c r="AV178" s="25">
-        <v>1000</v>
-      </c>
+      <c r="AV178" s="25"/>
       <c r="AW178" s="25"/>
       <c r="AX178" s="25"/>
       <c r="AY178" s="25"/>
@@ -23501,17 +23171,13 @@
       <c r="AU180" s="25"/>
       <c r="AV180" s="25"/>
       <c r="AW180" s="25"/>
-      <c r="AX180" s="25">
-        <v>2000</v>
-      </c>
+      <c r="AX180" s="25"/>
       <c r="AY180" s="25"/>
       <c r="AZ180" s="26"/>
       <c r="BA180" s="6"/>
       <c r="BB180" s="25"/>
       <c r="BC180" s="25"/>
-      <c r="BD180" s="25">
-        <v>2000</v>
-      </c>
+      <c r="BD180" s="25"/>
       <c r="BE180" s="25"/>
       <c r="BF180" s="25"/>
       <c r="BG180" s="6"/>
@@ -23709,17 +23375,13 @@
       <c r="AU182" s="25"/>
       <c r="AV182" s="25"/>
       <c r="AW182" s="25"/>
-      <c r="AX182" s="25">
-        <v>2500</v>
-      </c>
+      <c r="AX182" s="25"/>
       <c r="AY182" s="25"/>
       <c r="AZ182" s="26"/>
       <c r="BA182" s="6"/>
       <c r="BB182" s="25"/>
       <c r="BC182" s="25"/>
-      <c r="BD182" s="25">
-        <v>2500</v>
-      </c>
+      <c r="BD182" s="25"/>
       <c r="BE182" s="25"/>
       <c r="BF182" s="25"/>
       <c r="BG182" s="6"/>
@@ -23820,9 +23482,7 @@
       <c r="AU183" s="25"/>
       <c r="AV183" s="25"/>
       <c r="AW183" s="25"/>
-      <c r="AX183" s="25">
-        <v>3600</v>
-      </c>
+      <c r="AX183" s="25"/>
       <c r="AY183" s="25"/>
       <c r="AZ183" s="26"/>
       <c r="BA183" s="6"/>
@@ -24041,9 +23701,7 @@
       <c r="AS185" s="6"/>
       <c r="AT185" s="6"/>
       <c r="AU185" s="25"/>
-      <c r="AV185" s="25">
-        <v>30</v>
-      </c>
+      <c r="AV185" s="25"/>
       <c r="AW185" s="25"/>
       <c r="AX185" s="25"/>
       <c r="AY185" s="25"/>
@@ -24051,9 +23709,7 @@
       <c r="BA185" s="6"/>
       <c r="BB185" s="25"/>
       <c r="BC185" s="25"/>
-      <c r="BD185" s="25">
-        <v>25</v>
-      </c>
+      <c r="BD185" s="25"/>
       <c r="BE185" s="25"/>
       <c r="BF185" s="25"/>
       <c r="BG185" s="6"/>
@@ -24274,9 +23930,7 @@
       <c r="AV187" s="25"/>
       <c r="AW187" s="25"/>
       <c r="AX187" s="25"/>
-      <c r="AY187" s="25">
-        <v>250</v>
-      </c>
+      <c r="AY187" s="25"/>
       <c r="AZ187" s="26"/>
       <c r="BA187" s="6"/>
       <c r="BB187" s="25"/>
@@ -24499,9 +24153,7 @@
       <c r="BA189" s="6"/>
       <c r="BB189" s="25"/>
       <c r="BC189" s="25"/>
-      <c r="BD189" s="25">
-        <v>80</v>
-      </c>
+      <c r="BD189" s="25"/>
       <c r="BE189" s="25"/>
       <c r="BF189" s="25"/>
       <c r="BG189" s="6"/>
@@ -24717,9 +24369,7 @@
       <c r="AU191" s="25"/>
       <c r="AV191" s="25"/>
       <c r="AW191" s="25"/>
-      <c r="AX191" s="25">
-        <v>80</v>
-      </c>
+      <c r="AX191" s="25"/>
       <c r="AY191" s="25"/>
       <c r="AZ191" s="26"/>
       <c r="BA191" s="6"/>
@@ -24829,12 +24479,8 @@
       <c r="AT192" s="6"/>
       <c r="AU192" s="25"/>
       <c r="AV192" s="25"/>
-      <c r="AW192" s="25">
-        <v>50</v>
-      </c>
-      <c r="AX192" s="25">
-        <v>102</v>
-      </c>
+      <c r="AW192" s="25"/>
+      <c r="AX192" s="25"/>
       <c r="AY192" s="25"/>
       <c r="AZ192" s="26"/>
       <c r="BA192" s="6"/>
@@ -24945,9 +24591,7 @@
       <c r="AU193" s="25"/>
       <c r="AV193" s="25"/>
       <c r="AW193" s="25"/>
-      <c r="AX193" s="25">
-        <v>45</v>
-      </c>
+      <c r="AX193" s="25"/>
       <c r="AY193" s="25"/>
       <c r="AZ193" s="26"/>
       <c r="BA193" s="6"/>
@@ -25171,9 +24815,7 @@
       <c r="AV195" s="25"/>
       <c r="AW195" s="25"/>
       <c r="AX195" s="25"/>
-      <c r="AY195" s="25">
-        <v>48</v>
-      </c>
+      <c r="AY195" s="25"/>
       <c r="AZ195" s="26"/>
       <c r="BA195" s="6"/>
       <c r="BB195" s="25"/>
@@ -25522,10 +25164,7 @@
       <c r="AR198" s="25"/>
       <c r="AS198" s="6"/>
       <c r="AT198" s="6"/>
-      <c r="AU198" s="25">
-        <f>500+500</f>
-        <v>1000</v>
-      </c>
+      <c r="AU198" s="25"/>
       <c r="AV198" s="25"/>
       <c r="AW198" s="25"/>
       <c r="AX198" s="25"/>
@@ -26354,9 +25993,7 @@
       <c r="AU205" s="25"/>
       <c r="AV205" s="25"/>
       <c r="AW205" s="25"/>
-      <c r="AX205" s="25">
-        <v>500</v>
-      </c>
+      <c r="AX205" s="25"/>
       <c r="AY205" s="25"/>
       <c r="AZ205" s="26"/>
       <c r="BA205" s="6"/>
@@ -26470,9 +26107,7 @@
       <c r="AY206" s="25"/>
       <c r="AZ206" s="26"/>
       <c r="BA206" s="6"/>
-      <c r="BB206" s="25">
-        <v>296</v>
-      </c>
+      <c r="BB206" s="25"/>
       <c r="BC206" s="25"/>
       <c r="BD206" s="25"/>
       <c r="BE206" s="25"/>
@@ -26584,9 +26219,7 @@
       <c r="AY207" s="25"/>
       <c r="AZ207" s="26"/>
       <c r="BA207" s="6"/>
-      <c r="BB207" s="25">
-        <v>296</v>
-      </c>
+      <c r="BB207" s="25"/>
       <c r="BC207" s="25"/>
       <c r="BD207" s="25"/>
       <c r="BE207" s="25"/>
@@ -27827,9 +27460,7 @@
       <c r="AY218" s="25"/>
       <c r="AZ218" s="26"/>
       <c r="BA218" s="6"/>
-      <c r="BB218" s="25">
-        <v>42</v>
-      </c>
+      <c r="BB218" s="25"/>
       <c r="BC218" s="25"/>
       <c r="BD218" s="25"/>
       <c r="BE218" s="25"/>
@@ -28158,9 +27789,7 @@
       <c r="AU221" s="25"/>
       <c r="AV221" s="25"/>
       <c r="AW221" s="25"/>
-      <c r="AX221" s="25">
-        <v>40</v>
-      </c>
+      <c r="AX221" s="25"/>
       <c r="AY221" s="25"/>
       <c r="AZ221" s="26"/>
       <c r="BA221" s="6"/>
@@ -29935,9 +29564,7 @@
       <c r="AR237" s="25"/>
       <c r="AS237" s="6"/>
       <c r="AT237" s="6"/>
-      <c r="AU237" s="25">
-        <v>300</v>
-      </c>
+      <c r="AU237" s="25"/>
       <c r="AV237" s="25"/>
       <c r="AW237" s="25"/>
       <c r="AX237" s="25"/>
@@ -32371,474 +31998,435 @@
   </sheetData>
   <autoFilter ref="C2:D2" xr:uid="{CC412B54-366C-48C5-A561-3550BE0946A4}"/>
   <conditionalFormatting sqref="F38">
-    <cfRule type="cellIs" dxfId="118" priority="381" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="108" priority="381" operator="lessThanOrEqual">
       <formula>$G38</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="378" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="378" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="379" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="106" priority="379" operator="greaterThanOrEqual">
       <formula>$H38</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="380" operator="between">
+    <cfRule type="cellIs" dxfId="105" priority="380" operator="between">
       <formula>$G38</formula>
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24">
-    <cfRule type="cellIs" dxfId="114" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="156" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="155" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="103" priority="155" operator="lessThanOrEqual">
       <formula>$F24</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="154" operator="between">
+    <cfRule type="cellIs" dxfId="102" priority="154" operator="between">
       <formula>$F24</formula>
       <formula>$H24</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="153" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="101" priority="153" operator="greaterThanOrEqual">
       <formula>$G24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J65">
-    <cfRule type="cellIs" dxfId="110" priority="173" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="100" priority="173" operator="greaterThanOrEqual">
       <formula>$F65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="174" operator="between">
+    <cfRule type="cellIs" dxfId="99" priority="174" operator="between">
       <formula>$E65</formula>
       <formula>$G65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="175" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="98" priority="175" operator="lessThanOrEqual">
       <formula>$E65</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J66:J67 J70 M70:Q70 J99 M99:Q99 J203 M203:Q203">
-    <cfRule type="cellIs" dxfId="107" priority="178" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="97" priority="178" operator="lessThanOrEqual">
       <formula>$G66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="177" operator="between">
+    <cfRule type="cellIs" dxfId="96" priority="177" operator="between">
       <formula>$G66</formula>
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="176" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="95" priority="176" operator="greaterThanOrEqual">
       <formula>$H66</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J76">
-    <cfRule type="cellIs" dxfId="104" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="157" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J108 J130 M130:Q130 J132 M132:Q132">
-    <cfRule type="cellIs" dxfId="103" priority="163" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="93" priority="163" operator="lessThanOrEqual">
       <formula>$F108</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="162" operator="between">
+    <cfRule type="cellIs" dxfId="92" priority="162" operator="between">
       <formula>$F108</formula>
       <formula>$H108</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="161" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="91" priority="161" operator="greaterThanOrEqual">
       <formula>$G108</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J125">
-    <cfRule type="cellIs" dxfId="100" priority="168" operator="between">
+    <cfRule type="cellIs" dxfId="90" priority="168" operator="between">
       <formula>$F125</formula>
       <formula>$H125</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="167" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="89" priority="167" operator="greaterThanOrEqual">
       <formula>$G125</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="169" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="88" priority="169" operator="lessThanOrEqual">
       <formula>$F125</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J134">
-    <cfRule type="cellIs" dxfId="97" priority="172" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="87" priority="172" operator="lessThanOrEqual">
       <formula>$F134</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="171" operator="between">
+    <cfRule type="cellIs" dxfId="86" priority="171" operator="between">
       <formula>$F134</formula>
       <formula>$H134</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="170" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="85" priority="170" operator="greaterThanOrEqual">
       <formula>$G134</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J151:J152">
-    <cfRule type="cellIs" dxfId="94" priority="152" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="84" priority="152" operator="lessThanOrEqual">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="151" operator="between">
+    <cfRule type="cellIs" dxfId="83" priority="151" operator="between">
       <formula>#REF!</formula>
       <formula>$F151</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="150" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="82" priority="150" operator="greaterThanOrEqual">
       <formula>$E151</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="149" operator="equal">
       <formula>$F$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J163:J164">
-    <cfRule type="cellIs" dxfId="90" priority="148" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="80" priority="148" operator="lessThanOrEqual">
       <formula>$F163</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="147" operator="between">
+    <cfRule type="cellIs" dxfId="79" priority="147" operator="between">
       <formula>$F163</formula>
       <formula>$H163</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="146" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="78" priority="146" operator="greaterThanOrEqual">
       <formula>$G163</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J217">
-    <cfRule type="cellIs" dxfId="87" priority="166" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="77" priority="166" operator="lessThanOrEqual">
       <formula>$F217</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="164" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="76" priority="164" operator="greaterThanOrEqual">
       <formula>$G217</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="165" operator="between">
+    <cfRule type="cellIs" dxfId="75" priority="165" operator="between">
       <formula>$F217</formula>
       <formula>$H217</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J236">
-    <cfRule type="cellIs" dxfId="84" priority="158" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="74" priority="158" operator="greaterThanOrEqual">
       <formula>$G236</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="159" operator="between">
+    <cfRule type="cellIs" dxfId="73" priority="159" operator="between">
       <formula>$F236</formula>
       <formula>$H236</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="160" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="72" priority="160" operator="lessThanOrEqual">
       <formula>$F236</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M24:Q24">
-    <cfRule type="cellIs" dxfId="81" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="123" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="120" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="70" priority="120" operator="greaterThanOrEqual">
       <formula>$G24</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="121" operator="between">
+    <cfRule type="cellIs" dxfId="69" priority="121" operator="between">
       <formula>$F24</formula>
       <formula>$H24</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="122" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="68" priority="122" operator="lessThanOrEqual">
       <formula>$F24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M65:Q65">
-    <cfRule type="cellIs" dxfId="77" priority="141" operator="between">
+    <cfRule type="cellIs" dxfId="67" priority="141" operator="between">
       <formula>$E65</formula>
       <formula>$G65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="142" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="66" priority="142" operator="lessThanOrEqual">
       <formula>$E65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="140" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="65" priority="140" operator="greaterThanOrEqual">
       <formula>$F65</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M66:Q67">
-    <cfRule type="cellIs" dxfId="74" priority="78" operator="between">
+    <cfRule type="cellIs" dxfId="64" priority="78" operator="between">
       <formula>$G66</formula>
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="79" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="63" priority="79" operator="lessThanOrEqual">
       <formula>$G66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="77" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="62" priority="77" operator="greaterThanOrEqual">
       <formula>$H66</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M76:Q76">
-    <cfRule type="cellIs" dxfId="71" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="124" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M108:Q108">
-    <cfRule type="cellIs" dxfId="70" priority="130" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="60" priority="130" operator="lessThanOrEqual">
       <formula>$F108</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="129" operator="between">
+    <cfRule type="cellIs" dxfId="59" priority="129" operator="between">
       <formula>$F108</formula>
       <formula>$H108</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="128" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="58" priority="128" operator="greaterThanOrEqual">
       <formula>$G108</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M125:Q125">
-    <cfRule type="cellIs" dxfId="67" priority="135" operator="between">
+    <cfRule type="cellIs" dxfId="57" priority="135" operator="between">
       <formula>$F125</formula>
       <formula>$H125</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="134" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="56" priority="134" operator="greaterThanOrEqual">
       <formula>$G125</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="136" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="55" priority="136" operator="lessThanOrEqual">
       <formula>$F125</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M134:Q134">
-    <cfRule type="cellIs" dxfId="64" priority="138" operator="between">
+    <cfRule type="cellIs" dxfId="54" priority="138" operator="between">
       <formula>$F134</formula>
       <formula>$H134</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="139" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="53" priority="139" operator="lessThanOrEqual">
       <formula>$F134</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="137" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="52" priority="137" operator="greaterThanOrEqual">
       <formula>$G134</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M151:Q152">
-    <cfRule type="cellIs" dxfId="61" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="73" operator="equal">
       <formula>$F$1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="74" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="50" priority="74" operator="greaterThanOrEqual">
       <formula>$E151</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="75" operator="between">
+    <cfRule type="cellIs" dxfId="49" priority="75" operator="between">
       <formula>#REF!</formula>
       <formula>$F151</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="76" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="48" priority="76" operator="lessThanOrEqual">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M163:Q164">
-    <cfRule type="cellIs" dxfId="57" priority="70" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="47" priority="70" operator="greaterThanOrEqual">
       <formula>$G163</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="71" operator="between">
+    <cfRule type="cellIs" dxfId="46" priority="71" operator="between">
       <formula>$F163</formula>
       <formula>$H163</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="72" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="45" priority="72" operator="lessThanOrEqual">
       <formula>$F163</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M217:Q217">
-    <cfRule type="cellIs" dxfId="54" priority="131" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="44" priority="131" operator="greaterThanOrEqual">
       <formula>$G217</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="132" operator="between">
+    <cfRule type="cellIs" dxfId="43" priority="132" operator="between">
       <formula>$F217</formula>
       <formula>$H217</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="133" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="42" priority="133" operator="lessThanOrEqual">
       <formula>$F217</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M236:Q236">
-    <cfRule type="cellIs" dxfId="51" priority="125" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="41" priority="125" operator="greaterThanOrEqual">
       <formula>$G236</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="127" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="40" priority="127" operator="lessThanOrEqual">
       <formula>$F236</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="126" operator="between">
+    <cfRule type="cellIs" dxfId="39" priority="126" operator="between">
       <formula>$F236</formula>
       <formula>$H236</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T24:W24">
-    <cfRule type="cellIs" dxfId="48" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="44" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="43" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="37" priority="43" operator="lessThanOrEqual">
       <formula>$F24</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="41" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="36" priority="41" operator="greaterThanOrEqual">
       <formula>$G24</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="42" operator="between">
+    <cfRule type="cellIs" dxfId="35" priority="42" operator="between">
       <formula>$F24</formula>
       <formula>$H24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T65:W65">
-    <cfRule type="cellIs" dxfId="44" priority="61" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="34" priority="61" operator="greaterThanOrEqual">
       <formula>$F65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="63" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="33" priority="63" operator="lessThanOrEqual">
       <formula>$E65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="62" operator="between">
+    <cfRule type="cellIs" dxfId="32" priority="62" operator="between">
       <formula>$E65</formula>
       <formula>$G65</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T66:V67">
-    <cfRule type="cellIs" dxfId="41" priority="18" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="T66:W67">
+    <cfRule type="cellIs" dxfId="31" priority="8" operator="greaterThanOrEqual">
       <formula>$H66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="19" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="9" operator="between">
       <formula>$G66</formula>
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="20" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="29" priority="10" operator="lessThanOrEqual">
       <formula>$G66</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T70:W70 T99:W99 T203:W203">
-    <cfRule type="cellIs" dxfId="38" priority="67" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="28" priority="67" operator="greaterThanOrEqual">
       <formula>$H70</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="69" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="27" priority="69" operator="lessThanOrEqual">
       <formula>$G70</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="68" operator="between">
+    <cfRule type="cellIs" dxfId="26" priority="68" operator="between">
       <formula>$G70</formula>
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T76:W76">
-    <cfRule type="cellIs" dxfId="35" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="45" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T108:W108">
-    <cfRule type="cellIs" dxfId="34" priority="49" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="49" operator="greaterThanOrEqual">
       <formula>$G108</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="51" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="23" priority="51" operator="lessThanOrEqual">
       <formula>$F108</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="50" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="50" operator="between">
       <formula>$F108</formula>
       <formula>$H108</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T125:W125">
-    <cfRule type="cellIs" dxfId="31" priority="57" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="21" priority="57" operator="lessThanOrEqual">
       <formula>$F125</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="55" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="20" priority="55" operator="greaterThanOrEqual">
       <formula>$G125</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="56" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="56" operator="between">
       <formula>$F125</formula>
       <formula>$H125</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T130:W130 T132:W132">
-    <cfRule type="cellIs" dxfId="28" priority="65" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="65" operator="between">
       <formula>$F130</formula>
       <formula>$H130</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="66" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="17" priority="66" operator="lessThanOrEqual">
       <formula>$F130</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="64" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="64" operator="greaterThanOrEqual">
       <formula>$G130</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T134:W134">
-    <cfRule type="cellIs" dxfId="25" priority="58" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="15" priority="58" operator="greaterThanOrEqual">
       <formula>$G134</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="59" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="59" operator="between">
       <formula>$F134</formula>
       <formula>$H134</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="60" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="60" operator="lessThanOrEqual">
       <formula>$F134</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T151:V152">
-    <cfRule type="cellIs" dxfId="22" priority="17" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="T151:W152">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="lessThanOrEqual">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="16" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="between">
       <formula>#REF!</formula>
       <formula>$F151</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="greaterThanOrEqual">
       <formula>$E151</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>$F$1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T163:V164">
-    <cfRule type="cellIs" dxfId="18" priority="13" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="T163:W164">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="lessThanOrEqual">
       <formula>$F163</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThanOrEqual">
       <formula>$G163</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="between">
       <formula>$F163</formula>
       <formula>$H163</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T217:W217">
-    <cfRule type="cellIs" dxfId="15" priority="52" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="52" operator="greaterThanOrEqual">
       <formula>$G217</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="53" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="53" operator="between">
       <formula>$F217</formula>
       <formula>$H217</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="54" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="54" operator="lessThanOrEqual">
       <formula>$F217</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T236:W236">
-    <cfRule type="cellIs" dxfId="12" priority="46" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="46" operator="greaterThanOrEqual">
       <formula>$G236</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="47" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="47" operator="between">
       <formula>$F236</formula>
       <formula>$H236</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="48" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="48" operator="lessThanOrEqual">
       <formula>$F236</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W66:W67">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="greaterThanOrEqual">
-      <formula>$H66</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="between">
-      <formula>$G66</formula>
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="lessThanOrEqual">
-      <formula>$G66</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W151:W152">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>$F$1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThanOrEqual">
-      <formula>$E151</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="between">
-      <formula>#REF!</formula>
-      <formula>$F151</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThanOrEqual">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W163:W164">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
-      <formula>$G163</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="between">
-      <formula>$F163</formula>
-      <formula>$H163</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThanOrEqual">
-      <formula>$F163</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>